<commit_message>
dot in prices fix
</commit_message>
<xml_diff>
--- a/scripts/reports/My_ks2.xlsx
+++ b/scripts/reports/My_ks2.xlsx
@@ -326,7 +326,10 @@
     <t>${section1_relatedExpanses}</t>
   </si>
   <si>
-    <t>tttttttttttttttttttt</t>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
   <si>
     <t>Раздел 1. Система  автоматической пожарной сигнализации и оповещения и управления эвакуацией людей при пожаре (АПС и СОУЭ)</t>
@@ -335,13 +338,10 @@
     <t>название</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Раздел</t>
   </si>
   <si>
-    <t>tttttttttttttttttttttttttt</t>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ZZ51"/>
+  <dimension ref="A1:ZZ53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="ET38" sqref="ET38:FI38"/>
@@ -2843,7 +2843,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="72" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L13" s="73"/>
       <c r="M13" s="73"/>
@@ -3667,7 +3667,7 @@
       <c r="BV24" s="16"/>
       <c r="BW24" s="16"/>
       <c r="BX24" s="110">
-        <v>7.776000000000001</v>
+        <v>10.368</v>
       </c>
       <c r="BY24" s="111"/>
       <c r="BZ24" s="111"/>
@@ -4468,7 +4468,7 @@
     </row>
     <row r="30" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A30" s="77" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B30" s="78"/>
       <c r="C30" s="78"/>
@@ -4661,7 +4661,7 @@
       <c r="P31" s="84"/>
       <c r="Q31" s="85"/>
       <c r="R31" s="86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S31" s="87"/>
       <c r="T31" s="87"/>
@@ -4833,214 +4833,214 @@
       <c r="A32" s="80">
         <v>2</v>
       </c>
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="82"/>
       <c r="I32" s="83">
         <v>2</v>
       </c>
-      <c r="J32" s="84"/>
-      <c r="K32" s="84"/>
-      <c r="L32" s="84"/>
-      <c r="M32" s="84"/>
-      <c r="N32" s="84"/>
-      <c r="O32" s="84"/>
-      <c r="P32" s="84"/>
-      <c r="Q32" s="85"/>
       <c r="R32" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="S32" s="87"/>
-      <c r="T32" s="87"/>
-      <c r="U32" s="87"/>
-      <c r="V32" s="87"/>
-      <c r="W32" s="87"/>
-      <c r="X32" s="87"/>
-      <c r="Y32" s="87"/>
-      <c r="Z32" s="87"/>
-      <c r="AA32" s="87"/>
-      <c r="AB32" s="87"/>
-      <c r="AC32" s="87"/>
-      <c r="AD32" s="87"/>
-      <c r="AE32" s="87"/>
-      <c r="AF32" s="87"/>
-      <c r="AG32" s="87"/>
-      <c r="AH32" s="87"/>
-      <c r="AI32" s="87"/>
-      <c r="AJ32" s="87"/>
-      <c r="AK32" s="87"/>
-      <c r="AL32" s="87"/>
-      <c r="AM32" s="87"/>
-      <c r="AN32" s="87"/>
-      <c r="AO32" s="87"/>
-      <c r="AP32" s="87"/>
-      <c r="AQ32" s="87"/>
-      <c r="AR32" s="87"/>
-      <c r="AS32" s="87"/>
-      <c r="AT32" s="87"/>
-      <c r="AU32" s="87"/>
-      <c r="AV32" s="87"/>
-      <c r="AW32" s="87"/>
-      <c r="AX32" s="87"/>
-      <c r="AY32" s="87"/>
-      <c r="AZ32" s="87"/>
-      <c r="BA32" s="87"/>
-      <c r="BB32" s="87"/>
-      <c r="BC32" s="87"/>
-      <c r="BD32" s="87"/>
-      <c r="BE32" s="87"/>
-      <c r="BF32" s="87"/>
-      <c r="BG32" s="87"/>
-      <c r="BH32" s="87"/>
-      <c r="BI32" s="87"/>
-      <c r="BJ32" s="87"/>
-      <c r="BK32" s="87"/>
-      <c r="BL32" s="87"/>
-      <c r="BM32" s="87"/>
-      <c r="BN32" s="87"/>
-      <c r="BO32" s="87"/>
-      <c r="BP32" s="87"/>
-      <c r="BQ32" s="87"/>
-      <c r="BR32" s="87"/>
-      <c r="BS32" s="87"/>
-      <c r="BT32" s="87"/>
-      <c r="BU32" s="87"/>
-      <c r="BV32" s="87"/>
-      <c r="BW32" s="87"/>
-      <c r="BX32" s="87"/>
-      <c r="BY32" s="87"/>
-      <c r="BZ32" s="87"/>
-      <c r="CA32" s="87"/>
-      <c r="CB32" s="87"/>
-      <c r="CC32" s="87"/>
-      <c r="CD32" s="87"/>
-      <c r="CE32" s="87"/>
-      <c r="CF32" s="87"/>
-      <c r="CG32" s="87"/>
-      <c r="CH32" s="87"/>
-      <c r="CI32" s="87"/>
-      <c r="CJ32" s="87"/>
-      <c r="CK32" s="87"/>
-      <c r="CL32" s="87"/>
-      <c r="CM32" s="87"/>
-      <c r="CN32" s="87"/>
-      <c r="CO32" s="88"/>
-      <c r="CP32" s="89"/>
-      <c r="CQ32" s="90"/>
-      <c r="CR32" s="90"/>
-      <c r="CS32" s="90"/>
-      <c r="CT32" s="90"/>
-      <c r="CU32" s="90"/>
-      <c r="CV32" s="90"/>
-      <c r="CW32" s="90"/>
-      <c r="CX32" s="90"/>
-      <c r="CY32" s="90"/>
-      <c r="CZ32" s="90"/>
-      <c r="DA32" s="91"/>
+        <v>99</v>
+      </c>
       <c r="DB32" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="DC32" s="90"/>
-      <c r="DD32" s="90"/>
-      <c r="DE32" s="90"/>
-      <c r="DF32" s="90"/>
-      <c r="DG32" s="90"/>
-      <c r="DH32" s="90"/>
-      <c r="DI32" s="90"/>
-      <c r="DJ32" s="90"/>
-      <c r="DK32" s="90"/>
-      <c r="DL32" s="90"/>
-      <c r="DM32" s="91"/>
       <c r="DN32" s="92">
         <v>1</v>
       </c>
-      <c r="DO32" s="93"/>
-      <c r="DP32" s="93"/>
-      <c r="DQ32" s="93"/>
-      <c r="DR32" s="93"/>
-      <c r="DS32" s="93"/>
-      <c r="DT32" s="93"/>
-      <c r="DU32" s="93"/>
-      <c r="DV32" s="93"/>
-      <c r="DW32" s="93"/>
-      <c r="DX32" s="93"/>
-      <c r="DY32" s="93"/>
-      <c r="DZ32" s="93"/>
-      <c r="EA32" s="93"/>
-      <c r="EB32" s="93"/>
-      <c r="EC32" s="94"/>
       <c r="ED32" s="92">
         <v>1</v>
       </c>
-      <c r="EE32" s="93"/>
-      <c r="EF32" s="93"/>
-      <c r="EG32" s="93"/>
-      <c r="EH32" s="93"/>
-      <c r="EI32" s="93"/>
-      <c r="EJ32" s="93"/>
-      <c r="EK32" s="93"/>
-      <c r="EL32" s="93"/>
-      <c r="EM32" s="93"/>
-      <c r="EN32" s="93"/>
-      <c r="EO32" s="93"/>
-      <c r="EP32" s="93"/>
-      <c r="EQ32" s="93"/>
-      <c r="ER32" s="93"/>
-      <c r="ES32" s="94"/>
       <c r="ET32" s="92">
         <v>1</v>
-      </c>
-      <c r="EU32" s="93"/>
-      <c r="EV32" s="93"/>
-      <c r="EW32" s="93"/>
-      <c r="EX32" s="93"/>
-      <c r="EY32" s="93"/>
-      <c r="EZ32" s="93"/>
-      <c r="FA32" s="93"/>
-      <c r="FB32" s="93"/>
-      <c r="FC32" s="93"/>
-      <c r="FD32" s="93"/>
-      <c r="FE32" s="93"/>
-      <c r="FF32" s="93"/>
-      <c r="FG32" s="93"/>
-      <c r="FH32" s="93"/>
-      <c r="FI32" s="94"/>
-      <c r="ZG32" s="1">
-        <v>2</v>
-      </c>
-      <c r="ZH32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="ZI32" s="1"/>
-      <c r="ZZ32" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A33" s="80">
         <v>3</v>
       </c>
+      <c r="B33" s="81"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="82"/>
       <c r="I33" s="83">
         <v>3</v>
       </c>
+      <c r="J33" s="84"/>
+      <c r="K33" s="84"/>
+      <c r="L33" s="84"/>
+      <c r="M33" s="84"/>
+      <c r="N33" s="84"/>
+      <c r="O33" s="84"/>
+      <c r="P33" s="84"/>
+      <c r="Q33" s="85"/>
       <c r="R33" s="86" t="s">
-        <v>98</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="S33" s="87"/>
+      <c r="T33" s="87"/>
+      <c r="U33" s="87"/>
+      <c r="V33" s="87"/>
+      <c r="W33" s="87"/>
+      <c r="X33" s="87"/>
+      <c r="Y33" s="87"/>
+      <c r="Z33" s="87"/>
+      <c r="AA33" s="87"/>
+      <c r="AB33" s="87"/>
+      <c r="AC33" s="87"/>
+      <c r="AD33" s="87"/>
+      <c r="AE33" s="87"/>
+      <c r="AF33" s="87"/>
+      <c r="AG33" s="87"/>
+      <c r="AH33" s="87"/>
+      <c r="AI33" s="87"/>
+      <c r="AJ33" s="87"/>
+      <c r="AK33" s="87"/>
+      <c r="AL33" s="87"/>
+      <c r="AM33" s="87"/>
+      <c r="AN33" s="87"/>
+      <c r="AO33" s="87"/>
+      <c r="AP33" s="87"/>
+      <c r="AQ33" s="87"/>
+      <c r="AR33" s="87"/>
+      <c r="AS33" s="87"/>
+      <c r="AT33" s="87"/>
+      <c r="AU33" s="87"/>
+      <c r="AV33" s="87"/>
+      <c r="AW33" s="87"/>
+      <c r="AX33" s="87"/>
+      <c r="AY33" s="87"/>
+      <c r="AZ33" s="87"/>
+      <c r="BA33" s="87"/>
+      <c r="BB33" s="87"/>
+      <c r="BC33" s="87"/>
+      <c r="BD33" s="87"/>
+      <c r="BE33" s="87"/>
+      <c r="BF33" s="87"/>
+      <c r="BG33" s="87"/>
+      <c r="BH33" s="87"/>
+      <c r="BI33" s="87"/>
+      <c r="BJ33" s="87"/>
+      <c r="BK33" s="87"/>
+      <c r="BL33" s="87"/>
+      <c r="BM33" s="87"/>
+      <c r="BN33" s="87"/>
+      <c r="BO33" s="87"/>
+      <c r="BP33" s="87"/>
+      <c r="BQ33" s="87"/>
+      <c r="BR33" s="87"/>
+      <c r="BS33" s="87"/>
+      <c r="BT33" s="87"/>
+      <c r="BU33" s="87"/>
+      <c r="BV33" s="87"/>
+      <c r="BW33" s="87"/>
+      <c r="BX33" s="87"/>
+      <c r="BY33" s="87"/>
+      <c r="BZ33" s="87"/>
+      <c r="CA33" s="87"/>
+      <c r="CB33" s="87"/>
+      <c r="CC33" s="87"/>
+      <c r="CD33" s="87"/>
+      <c r="CE33" s="87"/>
+      <c r="CF33" s="87"/>
+      <c r="CG33" s="87"/>
+      <c r="CH33" s="87"/>
+      <c r="CI33" s="87"/>
+      <c r="CJ33" s="87"/>
+      <c r="CK33" s="87"/>
+      <c r="CL33" s="87"/>
+      <c r="CM33" s="87"/>
+      <c r="CN33" s="87"/>
+      <c r="CO33" s="88"/>
+      <c r="CP33" s="89"/>
+      <c r="CQ33" s="90"/>
+      <c r="CR33" s="90"/>
+      <c r="CS33" s="90"/>
+      <c r="CT33" s="90"/>
+      <c r="CU33" s="90"/>
+      <c r="CV33" s="90"/>
+      <c r="CW33" s="90"/>
+      <c r="CX33" s="90"/>
+      <c r="CY33" s="90"/>
+      <c r="CZ33" s="90"/>
+      <c r="DA33" s="91"/>
       <c r="DB33" s="89" t="s">
         <v>43</v>
       </c>
+      <c r="DC33" s="90"/>
+      <c r="DD33" s="90"/>
+      <c r="DE33" s="90"/>
+      <c r="DF33" s="90"/>
+      <c r="DG33" s="90"/>
+      <c r="DH33" s="90"/>
+      <c r="DI33" s="90"/>
+      <c r="DJ33" s="90"/>
+      <c r="DK33" s="90"/>
+      <c r="DL33" s="90"/>
+      <c r="DM33" s="91"/>
       <c r="DN33" s="92">
         <v>1</v>
       </c>
+      <c r="DO33" s="93"/>
+      <c r="DP33" s="93"/>
+      <c r="DQ33" s="93"/>
+      <c r="DR33" s="93"/>
+      <c r="DS33" s="93"/>
+      <c r="DT33" s="93"/>
+      <c r="DU33" s="93"/>
+      <c r="DV33" s="93"/>
+      <c r="DW33" s="93"/>
+      <c r="DX33" s="93"/>
+      <c r="DY33" s="93"/>
+      <c r="DZ33" s="93"/>
+      <c r="EA33" s="93"/>
+      <c r="EB33" s="93"/>
+      <c r="EC33" s="94"/>
       <c r="ED33" s="92">
         <v>1</v>
       </c>
+      <c r="EE33" s="93"/>
+      <c r="EF33" s="93"/>
+      <c r="EG33" s="93"/>
+      <c r="EH33" s="93"/>
+      <c r="EI33" s="93"/>
+      <c r="EJ33" s="93"/>
+      <c r="EK33" s="93"/>
+      <c r="EL33" s="93"/>
+      <c r="EM33" s="93"/>
+      <c r="EN33" s="93"/>
+      <c r="EO33" s="93"/>
+      <c r="EP33" s="93"/>
+      <c r="EQ33" s="93"/>
+      <c r="ER33" s="93"/>
+      <c r="ES33" s="94"/>
       <c r="ET33" s="92">
         <v>1</v>
+      </c>
+      <c r="EU33" s="93"/>
+      <c r="EV33" s="93"/>
+      <c r="EW33" s="93"/>
+      <c r="EX33" s="93"/>
+      <c r="EY33" s="93"/>
+      <c r="EZ33" s="93"/>
+      <c r="FA33" s="93"/>
+      <c r="FB33" s="93"/>
+      <c r="FC33" s="93"/>
+      <c r="FD33" s="93"/>
+      <c r="FE33" s="93"/>
+      <c r="FF33" s="93"/>
+      <c r="FG33" s="93"/>
+      <c r="FH33" s="93"/>
+      <c r="FI33" s="94"/>
+      <c r="ZG33" s="1">
+        <v>2</v>
+      </c>
+      <c r="ZH33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="ZI33" s="1"/>
+      <c r="ZZ33" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:702" x14ac:dyDescent="0.2">
@@ -5051,7 +5051,7 @@
         <v>4</v>
       </c>
       <c r="R34" s="86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="DB34" s="89" t="s">
         <v>43</v>
@@ -5204,8 +5204,8 @@
       <c r="EA35" s="97"/>
       <c r="EB35" s="97"/>
       <c r="EC35" s="98"/>
-      <c r="ED35" s="92" t="s">
-        <v>99</v>
+      <c r="ED35" s="92">
+        <v>0.32</v>
       </c>
       <c r="EE35" s="97"/>
       <c r="EF35" s="97"/>
@@ -5222,8 +5222,8 @@
       <c r="EQ35" s="97"/>
       <c r="ER35" s="97"/>
       <c r="ES35" s="98"/>
-      <c r="ET35" s="92" t="s">
-        <v>99</v>
+      <c r="ET35" s="92">
+        <v>0.32</v>
       </c>
       <c r="EU35" s="97"/>
       <c r="EV35" s="97"/>
@@ -5618,7 +5618,7 @@
       <c r="P38" s="84"/>
       <c r="Q38" s="85"/>
       <c r="R38" s="86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S38" s="87"/>
       <c r="T38" s="87"/>
@@ -5784,189 +5784,29 @@
       <c r="A39" s="80">
         <v>6</v>
       </c>
-      <c r="B39" s="81"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="82"/>
       <c r="I39" s="83">
         <v>6</v>
       </c>
-      <c r="J39" s="84"/>
-      <c r="K39" s="84"/>
-      <c r="L39" s="84"/>
-      <c r="M39" s="84"/>
-      <c r="N39" s="84"/>
-      <c r="O39" s="84"/>
-      <c r="P39" s="84"/>
-      <c r="Q39" s="85"/>
       <c r="R39" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="S39" s="87"/>
-      <c r="T39" s="87"/>
-      <c r="U39" s="87"/>
-      <c r="V39" s="87"/>
-      <c r="W39" s="87"/>
-      <c r="X39" s="87"/>
-      <c r="Y39" s="87"/>
-      <c r="Z39" s="87"/>
-      <c r="AA39" s="87"/>
-      <c r="AB39" s="87"/>
-      <c r="AC39" s="87"/>
-      <c r="AD39" s="87"/>
-      <c r="AE39" s="87"/>
-      <c r="AF39" s="87"/>
-      <c r="AG39" s="87"/>
-      <c r="AH39" s="87"/>
-      <c r="AI39" s="87"/>
-      <c r="AJ39" s="87"/>
-      <c r="AK39" s="87"/>
-      <c r="AL39" s="87"/>
-      <c r="AM39" s="87"/>
-      <c r="AN39" s="87"/>
-      <c r="AO39" s="87"/>
-      <c r="AP39" s="87"/>
-      <c r="AQ39" s="87"/>
-      <c r="AR39" s="87"/>
-      <c r="AS39" s="87"/>
-      <c r="AT39" s="87"/>
-      <c r="AU39" s="87"/>
-      <c r="AV39" s="87"/>
-      <c r="AW39" s="87"/>
-      <c r="AX39" s="87"/>
-      <c r="AY39" s="87"/>
-      <c r="AZ39" s="87"/>
-      <c r="BA39" s="87"/>
-      <c r="BB39" s="87"/>
-      <c r="BC39" s="87"/>
-      <c r="BD39" s="87"/>
-      <c r="BE39" s="87"/>
-      <c r="BF39" s="87"/>
-      <c r="BG39" s="87"/>
-      <c r="BH39" s="87"/>
-      <c r="BI39" s="87"/>
-      <c r="BJ39" s="87"/>
-      <c r="BK39" s="87"/>
-      <c r="BL39" s="87"/>
-      <c r="BM39" s="87"/>
-      <c r="BN39" s="87"/>
-      <c r="BO39" s="87"/>
-      <c r="BP39" s="87"/>
-      <c r="BQ39" s="87"/>
-      <c r="BR39" s="87"/>
-      <c r="BS39" s="87"/>
-      <c r="BT39" s="87"/>
-      <c r="BU39" s="87"/>
-      <c r="BV39" s="87"/>
-      <c r="BW39" s="87"/>
-      <c r="BX39" s="87"/>
-      <c r="BY39" s="87"/>
-      <c r="BZ39" s="87"/>
-      <c r="CA39" s="87"/>
-      <c r="CB39" s="87"/>
-      <c r="CC39" s="87"/>
-      <c r="CD39" s="87"/>
-      <c r="CE39" s="87"/>
-      <c r="CF39" s="87"/>
-      <c r="CG39" s="87"/>
-      <c r="CH39" s="87"/>
-      <c r="CI39" s="87"/>
-      <c r="CJ39" s="87"/>
-      <c r="CK39" s="87"/>
-      <c r="CL39" s="87"/>
-      <c r="CM39" s="87"/>
-      <c r="CN39" s="87"/>
-      <c r="CO39" s="88"/>
-      <c r="CP39" s="89"/>
-      <c r="CQ39" s="90"/>
-      <c r="CR39" s="90"/>
-      <c r="CS39" s="90"/>
-      <c r="CT39" s="90"/>
-      <c r="CU39" s="90"/>
-      <c r="CV39" s="90"/>
-      <c r="CW39" s="90"/>
-      <c r="CX39" s="90"/>
-      <c r="CY39" s="90"/>
-      <c r="CZ39" s="90"/>
-      <c r="DA39" s="91"/>
+        <v>99</v>
+      </c>
       <c r="DB39" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="DC39" s="90"/>
-      <c r="DD39" s="90"/>
-      <c r="DE39" s="90"/>
-      <c r="DF39" s="90"/>
-      <c r="DG39" s="90"/>
-      <c r="DH39" s="90"/>
-      <c r="DI39" s="90"/>
-      <c r="DJ39" s="90"/>
-      <c r="DK39" s="90"/>
-      <c r="DL39" s="90"/>
-      <c r="DM39" s="91"/>
       <c r="DN39" s="92">
         <v>1</v>
       </c>
-      <c r="DO39" s="93"/>
-      <c r="DP39" s="93"/>
-      <c r="DQ39" s="93"/>
-      <c r="DR39" s="93"/>
-      <c r="DS39" s="93"/>
-      <c r="DT39" s="93"/>
-      <c r="DU39" s="93"/>
-      <c r="DV39" s="93"/>
-      <c r="DW39" s="93"/>
-      <c r="DX39" s="93"/>
-      <c r="DY39" s="93"/>
-      <c r="DZ39" s="93"/>
-      <c r="EA39" s="93"/>
-      <c r="EB39" s="93"/>
-      <c r="EC39" s="94"/>
       <c r="ED39" s="92">
         <v>1</v>
       </c>
-      <c r="EE39" s="93"/>
-      <c r="EF39" s="93"/>
-      <c r="EG39" s="93"/>
-      <c r="EH39" s="93"/>
-      <c r="EI39" s="93"/>
-      <c r="EJ39" s="93"/>
-      <c r="EK39" s="93"/>
-      <c r="EL39" s="93"/>
-      <c r="EM39" s="93"/>
-      <c r="EN39" s="93"/>
-      <c r="EO39" s="93"/>
-      <c r="EP39" s="93"/>
-      <c r="EQ39" s="93"/>
-      <c r="ER39" s="93"/>
-      <c r="ES39" s="94"/>
       <c r="ET39" s="92">
         <v>1</v>
       </c>
-      <c r="EU39" s="93"/>
-      <c r="EV39" s="93"/>
-      <c r="EW39" s="93"/>
-      <c r="EX39" s="93"/>
-      <c r="EY39" s="93"/>
-      <c r="EZ39" s="93"/>
-      <c r="FA39" s="93"/>
-      <c r="FB39" s="93"/>
-      <c r="FC39" s="93"/>
-      <c r="FD39" s="93"/>
-      <c r="FE39" s="93"/>
-      <c r="FF39" s="93"/>
-      <c r="FG39" s="93"/>
-      <c r="FH39" s="93"/>
-      <c r="FI39" s="94"/>
-      <c r="ZG39" s="1"/>
-      <c r="ZH39" s="1"/>
-      <c r="ZI39" s="1"/>
-      <c r="ZZ39" s="1"/>
     </row>
     <row customHeight="1" ht="10.199999999999999" r="40" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="A40" s="80"/>
+      <c r="A40" s="80">
+        <v>7</v>
+      </c>
       <c r="B40" s="81"/>
       <c r="C40" s="81"/>
       <c r="D40" s="81"/>
@@ -5974,1360 +5814,1566 @@
       <c r="F40" s="81"/>
       <c r="G40" s="81"/>
       <c r="H40" s="82"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="81"/>
-      <c r="M40" s="81"/>
-      <c r="N40" s="81"/>
-      <c r="O40" s="81"/>
-      <c r="P40" s="81"/>
-      <c r="Q40" s="82"/>
+      <c r="I40" s="83">
+        <v>7</v>
+      </c>
+      <c r="J40" s="84"/>
+      <c r="K40" s="84"/>
+      <c r="L40" s="84"/>
+      <c r="M40" s="84"/>
+      <c r="N40" s="84"/>
+      <c r="O40" s="84"/>
+      <c r="P40" s="84"/>
+      <c r="Q40" s="85"/>
       <c r="R40" s="86" t="s">
-        <v>91</v>
-      </c>
-      <c r="S40" s="95"/>
-      <c r="T40" s="95"/>
-      <c r="U40" s="95"/>
-      <c r="V40" s="95"/>
-      <c r="W40" s="95"/>
-      <c r="X40" s="95"/>
-      <c r="Y40" s="95"/>
-      <c r="Z40" s="95"/>
-      <c r="AA40" s="95"/>
-      <c r="AB40" s="95"/>
-      <c r="AC40" s="95"/>
-      <c r="AD40" s="95"/>
-      <c r="AE40" s="95"/>
-      <c r="AF40" s="95"/>
-      <c r="AG40" s="95"/>
-      <c r="AH40" s="95"/>
-      <c r="AI40" s="95"/>
-      <c r="AJ40" s="95"/>
-      <c r="AK40" s="95"/>
-      <c r="AL40" s="95"/>
-      <c r="AM40" s="95"/>
-      <c r="AN40" s="95"/>
-      <c r="AO40" s="95"/>
-      <c r="AP40" s="95"/>
-      <c r="AQ40" s="95"/>
-      <c r="AR40" s="95"/>
-      <c r="AS40" s="95"/>
-      <c r="AT40" s="95"/>
-      <c r="AU40" s="95"/>
-      <c r="AV40" s="95"/>
-      <c r="AW40" s="95"/>
-      <c r="AX40" s="95"/>
-      <c r="AY40" s="95"/>
-      <c r="AZ40" s="95"/>
-      <c r="BA40" s="95"/>
-      <c r="BB40" s="95"/>
-      <c r="BC40" s="95"/>
-      <c r="BD40" s="95"/>
-      <c r="BE40" s="95"/>
-      <c r="BF40" s="95"/>
-      <c r="BG40" s="95"/>
-      <c r="BH40" s="95"/>
-      <c r="BI40" s="95"/>
-      <c r="BJ40" s="95"/>
-      <c r="BK40" s="95"/>
-      <c r="BL40" s="95"/>
-      <c r="BM40" s="95"/>
-      <c r="BN40" s="95"/>
-      <c r="BO40" s="95"/>
-      <c r="BP40" s="95"/>
-      <c r="BQ40" s="95"/>
-      <c r="BR40" s="95"/>
-      <c r="BS40" s="95"/>
-      <c r="BT40" s="95"/>
-      <c r="BU40" s="95"/>
-      <c r="BV40" s="95"/>
-      <c r="BW40" s="95"/>
-      <c r="BX40" s="95"/>
-      <c r="BY40" s="95"/>
-      <c r="BZ40" s="95"/>
-      <c r="CA40" s="95"/>
-      <c r="CB40" s="95"/>
-      <c r="CC40" s="95"/>
-      <c r="CD40" s="95"/>
-      <c r="CE40" s="95"/>
-      <c r="CF40" s="95"/>
-      <c r="CG40" s="95"/>
-      <c r="CH40" s="95"/>
-      <c r="CI40" s="95"/>
-      <c r="CJ40" s="95"/>
-      <c r="CK40" s="95"/>
-      <c r="CL40" s="95"/>
-      <c r="CM40" s="95"/>
-      <c r="CN40" s="95"/>
-      <c r="CO40" s="96"/>
+        <v>99</v>
+      </c>
+      <c r="S40" s="87"/>
+      <c r="T40" s="87"/>
+      <c r="U40" s="87"/>
+      <c r="V40" s="87"/>
+      <c r="W40" s="87"/>
+      <c r="X40" s="87"/>
+      <c r="Y40" s="87"/>
+      <c r="Z40" s="87"/>
+      <c r="AA40" s="87"/>
+      <c r="AB40" s="87"/>
+      <c r="AC40" s="87"/>
+      <c r="AD40" s="87"/>
+      <c r="AE40" s="87"/>
+      <c r="AF40" s="87"/>
+      <c r="AG40" s="87"/>
+      <c r="AH40" s="87"/>
+      <c r="AI40" s="87"/>
+      <c r="AJ40" s="87"/>
+      <c r="AK40" s="87"/>
+      <c r="AL40" s="87"/>
+      <c r="AM40" s="87"/>
+      <c r="AN40" s="87"/>
+      <c r="AO40" s="87"/>
+      <c r="AP40" s="87"/>
+      <c r="AQ40" s="87"/>
+      <c r="AR40" s="87"/>
+      <c r="AS40" s="87"/>
+      <c r="AT40" s="87"/>
+      <c r="AU40" s="87"/>
+      <c r="AV40" s="87"/>
+      <c r="AW40" s="87"/>
+      <c r="AX40" s="87"/>
+      <c r="AY40" s="87"/>
+      <c r="AZ40" s="87"/>
+      <c r="BA40" s="87"/>
+      <c r="BB40" s="87"/>
+      <c r="BC40" s="87"/>
+      <c r="BD40" s="87"/>
+      <c r="BE40" s="87"/>
+      <c r="BF40" s="87"/>
+      <c r="BG40" s="87"/>
+      <c r="BH40" s="87"/>
+      <c r="BI40" s="87"/>
+      <c r="BJ40" s="87"/>
+      <c r="BK40" s="87"/>
+      <c r="BL40" s="87"/>
+      <c r="BM40" s="87"/>
+      <c r="BN40" s="87"/>
+      <c r="BO40" s="87"/>
+      <c r="BP40" s="87"/>
+      <c r="BQ40" s="87"/>
+      <c r="BR40" s="87"/>
+      <c r="BS40" s="87"/>
+      <c r="BT40" s="87"/>
+      <c r="BU40" s="87"/>
+      <c r="BV40" s="87"/>
+      <c r="BW40" s="87"/>
+      <c r="BX40" s="87"/>
+      <c r="BY40" s="87"/>
+      <c r="BZ40" s="87"/>
+      <c r="CA40" s="87"/>
+      <c r="CB40" s="87"/>
+      <c r="CC40" s="87"/>
+      <c r="CD40" s="87"/>
+      <c r="CE40" s="87"/>
+      <c r="CF40" s="87"/>
+      <c r="CG40" s="87"/>
+      <c r="CH40" s="87"/>
+      <c r="CI40" s="87"/>
+      <c r="CJ40" s="87"/>
+      <c r="CK40" s="87"/>
+      <c r="CL40" s="87"/>
+      <c r="CM40" s="87"/>
+      <c r="CN40" s="87"/>
+      <c r="CO40" s="88"/>
       <c r="CP40" s="89"/>
-      <c r="CQ40" s="97"/>
-      <c r="CR40" s="97"/>
-      <c r="CS40" s="97"/>
-      <c r="CT40" s="97"/>
-      <c r="CU40" s="97"/>
-      <c r="CV40" s="97"/>
-      <c r="CW40" s="97"/>
-      <c r="CX40" s="97"/>
-      <c r="CY40" s="97"/>
-      <c r="CZ40" s="97"/>
-      <c r="DA40" s="98"/>
-      <c r="DB40" s="89"/>
-      <c r="DC40" s="97"/>
-      <c r="DD40" s="97"/>
-      <c r="DE40" s="97"/>
-      <c r="DF40" s="97"/>
-      <c r="DG40" s="97"/>
-      <c r="DH40" s="97"/>
-      <c r="DI40" s="97"/>
-      <c r="DJ40" s="97"/>
-      <c r="DK40" s="97"/>
-      <c r="DL40" s="97"/>
-      <c r="DM40" s="98"/>
+      <c r="CQ40" s="90"/>
+      <c r="CR40" s="90"/>
+      <c r="CS40" s="90"/>
+      <c r="CT40" s="90"/>
+      <c r="CU40" s="90"/>
+      <c r="CV40" s="90"/>
+      <c r="CW40" s="90"/>
+      <c r="CX40" s="90"/>
+      <c r="CY40" s="90"/>
+      <c r="CZ40" s="90"/>
+      <c r="DA40" s="91"/>
+      <c r="DB40" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="DC40" s="90"/>
+      <c r="DD40" s="90"/>
+      <c r="DE40" s="90"/>
+      <c r="DF40" s="90"/>
+      <c r="DG40" s="90"/>
+      <c r="DH40" s="90"/>
+      <c r="DI40" s="90"/>
+      <c r="DJ40" s="90"/>
+      <c r="DK40" s="90"/>
+      <c r="DL40" s="90"/>
+      <c r="DM40" s="91"/>
       <c r="DN40" s="92">
         <v>1</v>
       </c>
-      <c r="DO40" s="97"/>
-      <c r="DP40" s="97"/>
-      <c r="DQ40" s="97"/>
-      <c r="DR40" s="97"/>
-      <c r="DS40" s="97"/>
-      <c r="DT40" s="97"/>
-      <c r="DU40" s="97"/>
-      <c r="DV40" s="97"/>
-      <c r="DW40" s="97"/>
-      <c r="DX40" s="97"/>
-      <c r="DY40" s="97"/>
-      <c r="DZ40" s="97"/>
-      <c r="EA40" s="97"/>
-      <c r="EB40" s="97"/>
-      <c r="EC40" s="98"/>
-      <c r="ED40" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="EE40" s="97"/>
-      <c r="EF40" s="97"/>
-      <c r="EG40" s="97"/>
-      <c r="EH40" s="97"/>
-      <c r="EI40" s="97"/>
-      <c r="EJ40" s="97"/>
-      <c r="EK40" s="97"/>
-      <c r="EL40" s="97"/>
-      <c r="EM40" s="97"/>
-      <c r="EN40" s="97"/>
-      <c r="EO40" s="97"/>
-      <c r="EP40" s="97"/>
-      <c r="EQ40" s="97"/>
-      <c r="ER40" s="97"/>
-      <c r="ES40" s="98"/>
-      <c r="ET40" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="EU40" s="97"/>
-      <c r="EV40" s="97"/>
-      <c r="EW40" s="97"/>
-      <c r="EX40" s="97"/>
-      <c r="EY40" s="97"/>
-      <c r="EZ40" s="97"/>
-      <c r="FA40" s="97"/>
-      <c r="FB40" s="97"/>
-      <c r="FC40" s="97"/>
-      <c r="FD40" s="97"/>
-      <c r="FE40" s="97"/>
-      <c r="FF40" s="97"/>
-      <c r="FG40" s="97"/>
-      <c r="FH40" s="97"/>
-      <c r="FI40" s="98"/>
+      <c r="DO40" s="93"/>
+      <c r="DP40" s="93"/>
+      <c r="DQ40" s="93"/>
+      <c r="DR40" s="93"/>
+      <c r="DS40" s="93"/>
+      <c r="DT40" s="93"/>
+      <c r="DU40" s="93"/>
+      <c r="DV40" s="93"/>
+      <c r="DW40" s="93"/>
+      <c r="DX40" s="93"/>
+      <c r="DY40" s="93"/>
+      <c r="DZ40" s="93"/>
+      <c r="EA40" s="93"/>
+      <c r="EB40" s="93"/>
+      <c r="EC40" s="94"/>
+      <c r="ED40" s="92">
+        <v>1</v>
+      </c>
+      <c r="EE40" s="93"/>
+      <c r="EF40" s="93"/>
+      <c r="EG40" s="93"/>
+      <c r="EH40" s="93"/>
+      <c r="EI40" s="93"/>
+      <c r="EJ40" s="93"/>
+      <c r="EK40" s="93"/>
+      <c r="EL40" s="93"/>
+      <c r="EM40" s="93"/>
+      <c r="EN40" s="93"/>
+      <c r="EO40" s="93"/>
+      <c r="EP40" s="93"/>
+      <c r="EQ40" s="93"/>
+      <c r="ER40" s="93"/>
+      <c r="ES40" s="94"/>
+      <c r="ET40" s="92">
+        <v>1</v>
+      </c>
+      <c r="EU40" s="93"/>
+      <c r="EV40" s="93"/>
+      <c r="EW40" s="93"/>
+      <c r="EX40" s="93"/>
+      <c r="EY40" s="93"/>
+      <c r="EZ40" s="93"/>
+      <c r="FA40" s="93"/>
+      <c r="FB40" s="93"/>
+      <c r="FC40" s="93"/>
+      <c r="FD40" s="93"/>
+      <c r="FE40" s="93"/>
+      <c r="FF40" s="93"/>
+      <c r="FG40" s="93"/>
+      <c r="FH40" s="93"/>
+      <c r="FI40" s="94"/>
       <c r="ZG40" s="1"/>
       <c r="ZH40" s="1"/>
       <c r="ZI40" s="1"/>
       <c r="ZZ40" s="1"/>
     </row>
     <row customHeight="1" ht="10.199999999999999" r="41" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="A41" s="99" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="100"/>
-      <c r="C41" s="100"/>
-      <c r="D41" s="100"/>
-      <c r="E41" s="100"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="100"/>
-      <c r="H41" s="100"/>
-      <c r="I41" s="100"/>
-      <c r="J41" s="100"/>
-      <c r="K41" s="100"/>
-      <c r="L41" s="100"/>
-      <c r="M41" s="100"/>
-      <c r="N41" s="100"/>
-      <c r="O41" s="100"/>
-      <c r="P41" s="100"/>
-      <c r="Q41" s="100"/>
-      <c r="R41" s="100"/>
-      <c r="S41" s="100"/>
-      <c r="T41" s="100"/>
-      <c r="U41" s="100"/>
-      <c r="V41" s="100"/>
-      <c r="W41" s="100"/>
-      <c r="X41" s="100"/>
-      <c r="Y41" s="100"/>
-      <c r="Z41" s="100"/>
-      <c r="AA41" s="100"/>
-      <c r="AB41" s="100"/>
-      <c r="AC41" s="100"/>
-      <c r="AD41" s="100"/>
-      <c r="AE41" s="100"/>
-      <c r="AF41" s="100"/>
-      <c r="AG41" s="100"/>
-      <c r="AH41" s="100"/>
-      <c r="AI41" s="100"/>
-      <c r="AJ41" s="100"/>
-      <c r="AK41" s="100"/>
-      <c r="AL41" s="100"/>
-      <c r="AM41" s="100"/>
-      <c r="AN41" s="100"/>
-      <c r="AO41" s="100"/>
-      <c r="AP41" s="100"/>
-      <c r="AQ41" s="100"/>
-      <c r="AR41" s="100"/>
-      <c r="AS41" s="100"/>
-      <c r="AT41" s="100"/>
-      <c r="AU41" s="100"/>
-      <c r="AV41" s="100"/>
-      <c r="AW41" s="100"/>
-      <c r="AX41" s="100"/>
-      <c r="AY41" s="100"/>
-      <c r="AZ41" s="100"/>
-      <c r="BA41" s="100"/>
-      <c r="BB41" s="100"/>
-      <c r="BC41" s="100"/>
-      <c r="BD41" s="100"/>
-      <c r="BE41" s="100"/>
-      <c r="BF41" s="100"/>
-      <c r="BG41" s="100"/>
-      <c r="BH41" s="100"/>
-      <c r="BI41" s="100"/>
-      <c r="BJ41" s="100"/>
-      <c r="BK41" s="100"/>
-      <c r="BL41" s="100"/>
-      <c r="BM41" s="100"/>
-      <c r="BN41" s="100"/>
-      <c r="BO41" s="100"/>
-      <c r="BP41" s="100"/>
-      <c r="BQ41" s="100"/>
-      <c r="BR41" s="100"/>
-      <c r="BS41" s="100"/>
-      <c r="BT41" s="100"/>
-      <c r="BU41" s="100"/>
-      <c r="BV41" s="100"/>
-      <c r="BW41" s="100"/>
-      <c r="BX41" s="100"/>
-      <c r="BY41" s="100"/>
-      <c r="BZ41" s="100"/>
-      <c r="CA41" s="100"/>
-      <c r="CB41" s="100"/>
-      <c r="CC41" s="100"/>
-      <c r="CD41" s="100"/>
-      <c r="CE41" s="100"/>
-      <c r="CF41" s="100"/>
-      <c r="CG41" s="100"/>
-      <c r="CH41" s="100"/>
-      <c r="CI41" s="100"/>
-      <c r="CJ41" s="100"/>
-      <c r="CK41" s="100"/>
-      <c r="CL41" s="100"/>
-      <c r="CM41" s="100"/>
-      <c r="CN41" s="100"/>
-      <c r="CO41" s="100"/>
-      <c r="CP41" s="100"/>
-      <c r="CQ41" s="100"/>
-      <c r="CR41" s="100"/>
-      <c r="CS41" s="100"/>
-      <c r="CT41" s="100"/>
-      <c r="CU41" s="100"/>
-      <c r="CV41" s="100"/>
-      <c r="CW41" s="100"/>
-      <c r="CX41" s="100"/>
-      <c r="CY41" s="100"/>
-      <c r="CZ41" s="100"/>
-      <c r="DA41" s="100"/>
-      <c r="DB41" s="100"/>
-      <c r="DC41" s="100"/>
-      <c r="DD41" s="100"/>
-      <c r="DE41" s="100"/>
-      <c r="DF41" s="100"/>
-      <c r="DG41" s="100"/>
-      <c r="DH41" s="100"/>
-      <c r="DI41" s="100"/>
-      <c r="DJ41" s="100"/>
-      <c r="DK41" s="100"/>
-      <c r="DL41" s="100"/>
-      <c r="DM41" s="100"/>
-      <c r="DN41" s="100"/>
-      <c r="DO41" s="100"/>
-      <c r="DP41" s="100"/>
-      <c r="DQ41" s="100"/>
-      <c r="DR41" s="100"/>
-      <c r="DS41" s="100"/>
-      <c r="DT41" s="100"/>
-      <c r="DU41" s="100"/>
-      <c r="DV41" s="100"/>
-      <c r="DW41" s="100"/>
-      <c r="DX41" s="100"/>
-      <c r="DY41" s="100"/>
-      <c r="DZ41" s="100"/>
-      <c r="EA41" s="100"/>
-      <c r="EB41" s="100"/>
-      <c r="EC41" s="100"/>
-      <c r="ED41" s="100"/>
-      <c r="EE41" s="100"/>
-      <c r="EF41" s="100"/>
-      <c r="EG41" s="100"/>
-      <c r="EH41" s="100"/>
-      <c r="EI41" s="100"/>
-      <c r="EJ41" s="100"/>
-      <c r="EK41" s="100"/>
-      <c r="EL41" s="100"/>
-      <c r="EM41" s="100"/>
-      <c r="EN41" s="100"/>
-      <c r="EO41" s="100"/>
-      <c r="EP41" s="100"/>
-      <c r="EQ41" s="100"/>
-      <c r="ER41" s="100"/>
-      <c r="ES41" s="101"/>
-      <c r="ET41" s="102">
-        <v>2</v>
-      </c>
-      <c r="EU41" s="100"/>
-      <c r="EV41" s="100"/>
-      <c r="EW41" s="100"/>
-      <c r="EX41" s="100"/>
-      <c r="EY41" s="100"/>
-      <c r="EZ41" s="100"/>
-      <c r="FA41" s="100"/>
-      <c r="FB41" s="100"/>
-      <c r="FC41" s="100"/>
-      <c r="FD41" s="100"/>
-      <c r="FE41" s="100"/>
-      <c r="FF41" s="100"/>
-      <c r="FG41" s="100"/>
-      <c r="FH41" s="100"/>
-      <c r="FI41" s="101"/>
+      <c r="A41" s="80">
+        <v>8</v>
+      </c>
+      <c r="I41" s="83">
+        <v>8</v>
+      </c>
+      <c r="R41" s="86" t="s">
+        <v>99</v>
+      </c>
+      <c r="DB41" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="DN41" s="92">
+        <v>1</v>
+      </c>
+      <c r="ED41" s="92">
+        <v>1</v>
+      </c>
+      <c r="ET41" s="92">
+        <v>1</v>
+      </c>
     </row>
     <row customHeight="1" ht="10.199999999999999" r="42" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="A42" s="103"/>
-      <c r="B42" s="103"/>
-      <c r="C42" s="103"/>
-      <c r="D42" s="103"/>
-      <c r="E42" s="103"/>
-      <c r="F42" s="103"/>
-      <c r="G42" s="103"/>
-      <c r="H42" s="103"/>
-      <c r="I42" s="103"/>
-      <c r="J42" s="103"/>
-      <c r="K42" s="103"/>
-      <c r="L42" s="103"/>
-      <c r="M42" s="103"/>
-      <c r="N42" s="103"/>
-      <c r="O42" s="103"/>
-      <c r="P42" s="103"/>
-      <c r="Q42" s="103"/>
-      <c r="R42" s="103"/>
-      <c r="S42" s="103"/>
-      <c r="T42" s="103"/>
-      <c r="U42" s="103"/>
-      <c r="V42" s="103"/>
-      <c r="W42" s="103"/>
-      <c r="X42" s="103"/>
-      <c r="Y42" s="103"/>
-      <c r="Z42" s="103"/>
-      <c r="AA42" s="103"/>
-      <c r="AB42" s="103"/>
-      <c r="AC42" s="103"/>
-      <c r="AD42" s="103"/>
-      <c r="AE42" s="103"/>
-      <c r="AF42" s="103"/>
-      <c r="AG42" s="103"/>
-      <c r="AH42" s="103"/>
-      <c r="AI42" s="103"/>
-      <c r="AJ42" s="103"/>
-      <c r="AK42" s="103"/>
-      <c r="AL42" s="103"/>
-      <c r="AM42" s="103"/>
-      <c r="AN42" s="103"/>
-      <c r="AO42" s="103"/>
-      <c r="AP42" s="103"/>
-      <c r="AQ42" s="103"/>
-      <c r="AR42" s="103"/>
-      <c r="AS42" s="103"/>
-      <c r="AT42" s="103"/>
-      <c r="AU42" s="103"/>
-      <c r="AV42" s="103"/>
-      <c r="AW42" s="103"/>
-      <c r="AX42" s="103"/>
-      <c r="AY42" s="103"/>
-      <c r="AZ42" s="103"/>
-      <c r="BA42" s="103"/>
-      <c r="BB42" s="103"/>
-      <c r="BC42" s="103"/>
-      <c r="BD42" s="103"/>
-      <c r="BE42" s="103"/>
-      <c r="BF42" s="103"/>
-      <c r="BG42" s="103"/>
-      <c r="BH42" s="103"/>
-      <c r="BI42" s="103"/>
-      <c r="BJ42" s="103"/>
-      <c r="BK42" s="103"/>
-      <c r="BL42" s="103"/>
-      <c r="BM42" s="103"/>
-      <c r="BN42" s="103"/>
-      <c r="BO42" s="103"/>
-      <c r="BP42" s="103"/>
-      <c r="BQ42" s="103"/>
-      <c r="BR42" s="103"/>
-      <c r="BS42" s="103"/>
-      <c r="BT42" s="103"/>
-      <c r="BU42" s="103"/>
-      <c r="BV42" s="103"/>
-      <c r="BW42" s="103"/>
-      <c r="BX42" s="103"/>
-      <c r="BY42" s="103"/>
-      <c r="BZ42" s="103"/>
-      <c r="CA42" s="103"/>
-      <c r="CB42" s="103"/>
-      <c r="CC42" s="103"/>
-      <c r="CD42" s="103"/>
-      <c r="CE42" s="103"/>
-      <c r="CF42" s="103"/>
-      <c r="CG42" s="103"/>
-      <c r="CH42" s="103"/>
-      <c r="CI42" s="103"/>
-      <c r="CJ42" s="103"/>
-      <c r="CK42" s="103"/>
-      <c r="CL42" s="103"/>
-      <c r="CM42" s="103"/>
-      <c r="CN42" s="103"/>
-      <c r="CO42" s="103"/>
-      <c r="CP42" s="104" t="s">
+      <c r="A42" s="80"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="81"/>
+      <c r="G42" s="81"/>
+      <c r="H42" s="82"/>
+      <c r="I42" s="83"/>
+      <c r="J42" s="81"/>
+      <c r="K42" s="81"/>
+      <c r="L42" s="81"/>
+      <c r="M42" s="81"/>
+      <c r="N42" s="81"/>
+      <c r="O42" s="81"/>
+      <c r="P42" s="81"/>
+      <c r="Q42" s="82"/>
+      <c r="R42" s="86" t="s">
+        <v>91</v>
+      </c>
+      <c r="S42" s="95"/>
+      <c r="T42" s="95"/>
+      <c r="U42" s="95"/>
+      <c r="V42" s="95"/>
+      <c r="W42" s="95"/>
+      <c r="X42" s="95"/>
+      <c r="Y42" s="95"/>
+      <c r="Z42" s="95"/>
+      <c r="AA42" s="95"/>
+      <c r="AB42" s="95"/>
+      <c r="AC42" s="95"/>
+      <c r="AD42" s="95"/>
+      <c r="AE42" s="95"/>
+      <c r="AF42" s="95"/>
+      <c r="AG42" s="95"/>
+      <c r="AH42" s="95"/>
+      <c r="AI42" s="95"/>
+      <c r="AJ42" s="95"/>
+      <c r="AK42" s="95"/>
+      <c r="AL42" s="95"/>
+      <c r="AM42" s="95"/>
+      <c r="AN42" s="95"/>
+      <c r="AO42" s="95"/>
+      <c r="AP42" s="95"/>
+      <c r="AQ42" s="95"/>
+      <c r="AR42" s="95"/>
+      <c r="AS42" s="95"/>
+      <c r="AT42" s="95"/>
+      <c r="AU42" s="95"/>
+      <c r="AV42" s="95"/>
+      <c r="AW42" s="95"/>
+      <c r="AX42" s="95"/>
+      <c r="AY42" s="95"/>
+      <c r="AZ42" s="95"/>
+      <c r="BA42" s="95"/>
+      <c r="BB42" s="95"/>
+      <c r="BC42" s="95"/>
+      <c r="BD42" s="95"/>
+      <c r="BE42" s="95"/>
+      <c r="BF42" s="95"/>
+      <c r="BG42" s="95"/>
+      <c r="BH42" s="95"/>
+      <c r="BI42" s="95"/>
+      <c r="BJ42" s="95"/>
+      <c r="BK42" s="95"/>
+      <c r="BL42" s="95"/>
+      <c r="BM42" s="95"/>
+      <c r="BN42" s="95"/>
+      <c r="BO42" s="95"/>
+      <c r="BP42" s="95"/>
+      <c r="BQ42" s="95"/>
+      <c r="BR42" s="95"/>
+      <c r="BS42" s="95"/>
+      <c r="BT42" s="95"/>
+      <c r="BU42" s="95"/>
+      <c r="BV42" s="95"/>
+      <c r="BW42" s="95"/>
+      <c r="BX42" s="95"/>
+      <c r="BY42" s="95"/>
+      <c r="BZ42" s="95"/>
+      <c r="CA42" s="95"/>
+      <c r="CB42" s="95"/>
+      <c r="CC42" s="95"/>
+      <c r="CD42" s="95"/>
+      <c r="CE42" s="95"/>
+      <c r="CF42" s="95"/>
+      <c r="CG42" s="95"/>
+      <c r="CH42" s="95"/>
+      <c r="CI42" s="95"/>
+      <c r="CJ42" s="95"/>
+      <c r="CK42" s="95"/>
+      <c r="CL42" s="95"/>
+      <c r="CM42" s="95"/>
+      <c r="CN42" s="95"/>
+      <c r="CO42" s="96"/>
+      <c r="CP42" s="89"/>
+      <c r="CQ42" s="97"/>
+      <c r="CR42" s="97"/>
+      <c r="CS42" s="97"/>
+      <c r="CT42" s="97"/>
+      <c r="CU42" s="97"/>
+      <c r="CV42" s="97"/>
+      <c r="CW42" s="97"/>
+      <c r="CX42" s="97"/>
+      <c r="CY42" s="97"/>
+      <c r="CZ42" s="97"/>
+      <c r="DA42" s="98"/>
+      <c r="DB42" s="89"/>
+      <c r="DC42" s="97"/>
+      <c r="DD42" s="97"/>
+      <c r="DE42" s="97"/>
+      <c r="DF42" s="97"/>
+      <c r="DG42" s="97"/>
+      <c r="DH42" s="97"/>
+      <c r="DI42" s="97"/>
+      <c r="DJ42" s="97"/>
+      <c r="DK42" s="97"/>
+      <c r="DL42" s="97"/>
+      <c r="DM42" s="98"/>
+      <c r="DN42" s="92">
+        <v>1</v>
+      </c>
+      <c r="DO42" s="97"/>
+      <c r="DP42" s="97"/>
+      <c r="DQ42" s="97"/>
+      <c r="DR42" s="97"/>
+      <c r="DS42" s="97"/>
+      <c r="DT42" s="97"/>
+      <c r="DU42" s="97"/>
+      <c r="DV42" s="97"/>
+      <c r="DW42" s="97"/>
+      <c r="DX42" s="97"/>
+      <c r="DY42" s="97"/>
+      <c r="DZ42" s="97"/>
+      <c r="EA42" s="97"/>
+      <c r="EB42" s="97"/>
+      <c r="EC42" s="98"/>
+      <c r="ED42" s="92">
+        <v>0.32</v>
+      </c>
+      <c r="EE42" s="97"/>
+      <c r="EF42" s="97"/>
+      <c r="EG42" s="97"/>
+      <c r="EH42" s="97"/>
+      <c r="EI42" s="97"/>
+      <c r="EJ42" s="97"/>
+      <c r="EK42" s="97"/>
+      <c r="EL42" s="97"/>
+      <c r="EM42" s="97"/>
+      <c r="EN42" s="97"/>
+      <c r="EO42" s="97"/>
+      <c r="EP42" s="97"/>
+      <c r="EQ42" s="97"/>
+      <c r="ER42" s="97"/>
+      <c r="ES42" s="98"/>
+      <c r="ET42" s="92">
+        <v>0.32</v>
+      </c>
+      <c r="EU42" s="97"/>
+      <c r="EV42" s="97"/>
+      <c r="EW42" s="97"/>
+      <c r="EX42" s="97"/>
+      <c r="EY42" s="97"/>
+      <c r="EZ42" s="97"/>
+      <c r="FA42" s="97"/>
+      <c r="FB42" s="97"/>
+      <c r="FC42" s="97"/>
+      <c r="FD42" s="97"/>
+      <c r="FE42" s="97"/>
+      <c r="FF42" s="97"/>
+      <c r="FG42" s="97"/>
+      <c r="FH42" s="97"/>
+      <c r="FI42" s="98"/>
+      <c r="ZG42" s="1"/>
+      <c r="ZH42" s="1"/>
+      <c r="ZI42" s="1"/>
+      <c r="ZZ42" s="1"/>
+    </row>
+    <row customHeight="1" ht="10.199999999999999" r="43" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="A43" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="100"/>
+      <c r="C43" s="100"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="100"/>
+      <c r="F43" s="100"/>
+      <c r="G43" s="100"/>
+      <c r="H43" s="100"/>
+      <c r="I43" s="100"/>
+      <c r="J43" s="100"/>
+      <c r="K43" s="100"/>
+      <c r="L43" s="100"/>
+      <c r="M43" s="100"/>
+      <c r="N43" s="100"/>
+      <c r="O43" s="100"/>
+      <c r="P43" s="100"/>
+      <c r="Q43" s="100"/>
+      <c r="R43" s="100"/>
+      <c r="S43" s="100"/>
+      <c r="T43" s="100"/>
+      <c r="U43" s="100"/>
+      <c r="V43" s="100"/>
+      <c r="W43" s="100"/>
+      <c r="X43" s="100"/>
+      <c r="Y43" s="100"/>
+      <c r="Z43" s="100"/>
+      <c r="AA43" s="100"/>
+      <c r="AB43" s="100"/>
+      <c r="AC43" s="100"/>
+      <c r="AD43" s="100"/>
+      <c r="AE43" s="100"/>
+      <c r="AF43" s="100"/>
+      <c r="AG43" s="100"/>
+      <c r="AH43" s="100"/>
+      <c r="AI43" s="100"/>
+      <c r="AJ43" s="100"/>
+      <c r="AK43" s="100"/>
+      <c r="AL43" s="100"/>
+      <c r="AM43" s="100"/>
+      <c r="AN43" s="100"/>
+      <c r="AO43" s="100"/>
+      <c r="AP43" s="100"/>
+      <c r="AQ43" s="100"/>
+      <c r="AR43" s="100"/>
+      <c r="AS43" s="100"/>
+      <c r="AT43" s="100"/>
+      <c r="AU43" s="100"/>
+      <c r="AV43" s="100"/>
+      <c r="AW43" s="100"/>
+      <c r="AX43" s="100"/>
+      <c r="AY43" s="100"/>
+      <c r="AZ43" s="100"/>
+      <c r="BA43" s="100"/>
+      <c r="BB43" s="100"/>
+      <c r="BC43" s="100"/>
+      <c r="BD43" s="100"/>
+      <c r="BE43" s="100"/>
+      <c r="BF43" s="100"/>
+      <c r="BG43" s="100"/>
+      <c r="BH43" s="100"/>
+      <c r="BI43" s="100"/>
+      <c r="BJ43" s="100"/>
+      <c r="BK43" s="100"/>
+      <c r="BL43" s="100"/>
+      <c r="BM43" s="100"/>
+      <c r="BN43" s="100"/>
+      <c r="BO43" s="100"/>
+      <c r="BP43" s="100"/>
+      <c r="BQ43" s="100"/>
+      <c r="BR43" s="100"/>
+      <c r="BS43" s="100"/>
+      <c r="BT43" s="100"/>
+      <c r="BU43" s="100"/>
+      <c r="BV43" s="100"/>
+      <c r="BW43" s="100"/>
+      <c r="BX43" s="100"/>
+      <c r="BY43" s="100"/>
+      <c r="BZ43" s="100"/>
+      <c r="CA43" s="100"/>
+      <c r="CB43" s="100"/>
+      <c r="CC43" s="100"/>
+      <c r="CD43" s="100"/>
+      <c r="CE43" s="100"/>
+      <c r="CF43" s="100"/>
+      <c r="CG43" s="100"/>
+      <c r="CH43" s="100"/>
+      <c r="CI43" s="100"/>
+      <c r="CJ43" s="100"/>
+      <c r="CK43" s="100"/>
+      <c r="CL43" s="100"/>
+      <c r="CM43" s="100"/>
+      <c r="CN43" s="100"/>
+      <c r="CO43" s="100"/>
+      <c r="CP43" s="100"/>
+      <c r="CQ43" s="100"/>
+      <c r="CR43" s="100"/>
+      <c r="CS43" s="100"/>
+      <c r="CT43" s="100"/>
+      <c r="CU43" s="100"/>
+      <c r="CV43" s="100"/>
+      <c r="CW43" s="100"/>
+      <c r="CX43" s="100"/>
+      <c r="CY43" s="100"/>
+      <c r="CZ43" s="100"/>
+      <c r="DA43" s="100"/>
+      <c r="DB43" s="100"/>
+      <c r="DC43" s="100"/>
+      <c r="DD43" s="100"/>
+      <c r="DE43" s="100"/>
+      <c r="DF43" s="100"/>
+      <c r="DG43" s="100"/>
+      <c r="DH43" s="100"/>
+      <c r="DI43" s="100"/>
+      <c r="DJ43" s="100"/>
+      <c r="DK43" s="100"/>
+      <c r="DL43" s="100"/>
+      <c r="DM43" s="100"/>
+      <c r="DN43" s="100"/>
+      <c r="DO43" s="100"/>
+      <c r="DP43" s="100"/>
+      <c r="DQ43" s="100"/>
+      <c r="DR43" s="100"/>
+      <c r="DS43" s="100"/>
+      <c r="DT43" s="100"/>
+      <c r="DU43" s="100"/>
+      <c r="DV43" s="100"/>
+      <c r="DW43" s="100"/>
+      <c r="DX43" s="100"/>
+      <c r="DY43" s="100"/>
+      <c r="DZ43" s="100"/>
+      <c r="EA43" s="100"/>
+      <c r="EB43" s="100"/>
+      <c r="EC43" s="100"/>
+      <c r="ED43" s="100"/>
+      <c r="EE43" s="100"/>
+      <c r="EF43" s="100"/>
+      <c r="EG43" s="100"/>
+      <c r="EH43" s="100"/>
+      <c r="EI43" s="100"/>
+      <c r="EJ43" s="100"/>
+      <c r="EK43" s="100"/>
+      <c r="EL43" s="100"/>
+      <c r="EM43" s="100"/>
+      <c r="EN43" s="100"/>
+      <c r="EO43" s="100"/>
+      <c r="EP43" s="100"/>
+      <c r="EQ43" s="100"/>
+      <c r="ER43" s="100"/>
+      <c r="ES43" s="101"/>
+      <c r="ET43" s="102">
+        <v>4</v>
+      </c>
+      <c r="EU43" s="100"/>
+      <c r="EV43" s="100"/>
+      <c r="EW43" s="100"/>
+      <c r="EX43" s="100"/>
+      <c r="EY43" s="100"/>
+      <c r="EZ43" s="100"/>
+      <c r="FA43" s="100"/>
+      <c r="FB43" s="100"/>
+      <c r="FC43" s="100"/>
+      <c r="FD43" s="100"/>
+      <c r="FE43" s="100"/>
+      <c r="FF43" s="100"/>
+      <c r="FG43" s="100"/>
+      <c r="FH43" s="100"/>
+      <c r="FI43" s="101"/>
+    </row>
+    <row customHeight="1" ht="10.199999999999999" r="44" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="A44" s="103"/>
+      <c r="B44" s="103"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="103"/>
+      <c r="E44" s="103"/>
+      <c r="F44" s="103"/>
+      <c r="G44" s="103"/>
+      <c r="H44" s="103"/>
+      <c r="I44" s="103"/>
+      <c r="J44" s="103"/>
+      <c r="K44" s="103"/>
+      <c r="L44" s="103"/>
+      <c r="M44" s="103"/>
+      <c r="N44" s="103"/>
+      <c r="O44" s="103"/>
+      <c r="P44" s="103"/>
+      <c r="Q44" s="103"/>
+      <c r="R44" s="103"/>
+      <c r="S44" s="103"/>
+      <c r="T44" s="103"/>
+      <c r="U44" s="103"/>
+      <c r="V44" s="103"/>
+      <c r="W44" s="103"/>
+      <c r="X44" s="103"/>
+      <c r="Y44" s="103"/>
+      <c r="Z44" s="103"/>
+      <c r="AA44" s="103"/>
+      <c r="AB44" s="103"/>
+      <c r="AC44" s="103"/>
+      <c r="AD44" s="103"/>
+      <c r="AE44" s="103"/>
+      <c r="AF44" s="103"/>
+      <c r="AG44" s="103"/>
+      <c r="AH44" s="103"/>
+      <c r="AI44" s="103"/>
+      <c r="AJ44" s="103"/>
+      <c r="AK44" s="103"/>
+      <c r="AL44" s="103"/>
+      <c r="AM44" s="103"/>
+      <c r="AN44" s="103"/>
+      <c r="AO44" s="103"/>
+      <c r="AP44" s="103"/>
+      <c r="AQ44" s="103"/>
+      <c r="AR44" s="103"/>
+      <c r="AS44" s="103"/>
+      <c r="AT44" s="103"/>
+      <c r="AU44" s="103"/>
+      <c r="AV44" s="103"/>
+      <c r="AW44" s="103"/>
+      <c r="AX44" s="103"/>
+      <c r="AY44" s="103"/>
+      <c r="AZ44" s="103"/>
+      <c r="BA44" s="103"/>
+      <c r="BB44" s="103"/>
+      <c r="BC44" s="103"/>
+      <c r="BD44" s="103"/>
+      <c r="BE44" s="103"/>
+      <c r="BF44" s="103"/>
+      <c r="BG44" s="103"/>
+      <c r="BH44" s="103"/>
+      <c r="BI44" s="103"/>
+      <c r="BJ44" s="103"/>
+      <c r="BK44" s="103"/>
+      <c r="BL44" s="103"/>
+      <c r="BM44" s="103"/>
+      <c r="BN44" s="103"/>
+      <c r="BO44" s="103"/>
+      <c r="BP44" s="103"/>
+      <c r="BQ44" s="103"/>
+      <c r="BR44" s="103"/>
+      <c r="BS44" s="103"/>
+      <c r="BT44" s="103"/>
+      <c r="BU44" s="103"/>
+      <c r="BV44" s="103"/>
+      <c r="BW44" s="103"/>
+      <c r="BX44" s="103"/>
+      <c r="BY44" s="103"/>
+      <c r="BZ44" s="103"/>
+      <c r="CA44" s="103"/>
+      <c r="CB44" s="103"/>
+      <c r="CC44" s="103"/>
+      <c r="CD44" s="103"/>
+      <c r="CE44" s="103"/>
+      <c r="CF44" s="103"/>
+      <c r="CG44" s="103"/>
+      <c r="CH44" s="103"/>
+      <c r="CI44" s="103"/>
+      <c r="CJ44" s="103"/>
+      <c r="CK44" s="103"/>
+      <c r="CL44" s="103"/>
+      <c r="CM44" s="103"/>
+      <c r="CN44" s="103"/>
+      <c r="CO44" s="103"/>
+      <c r="CP44" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="CQ42" s="104"/>
-      <c r="CR42" s="104"/>
-      <c r="CS42" s="104"/>
-      <c r="CT42" s="104"/>
-      <c r="CU42" s="104"/>
-      <c r="CV42" s="104"/>
-      <c r="CW42" s="104"/>
-      <c r="CX42" s="104"/>
-      <c r="CY42" s="104"/>
-      <c r="CZ42" s="104"/>
-      <c r="DA42" s="104"/>
-      <c r="DB42" s="104"/>
-      <c r="DC42" s="104"/>
-      <c r="DD42" s="104"/>
-      <c r="DE42" s="104"/>
-      <c r="DF42" s="104"/>
-      <c r="DG42" s="104"/>
-      <c r="DH42" s="104"/>
-      <c r="DI42" s="104"/>
-      <c r="DJ42" s="104"/>
-      <c r="DK42" s="104"/>
-      <c r="DL42" s="104"/>
-      <c r="DM42" s="104"/>
-      <c r="DN42" s="105" t="s">
+      <c r="CQ44" s="104"/>
+      <c r="CR44" s="104"/>
+      <c r="CS44" s="104"/>
+      <c r="CT44" s="104"/>
+      <c r="CU44" s="104"/>
+      <c r="CV44" s="104"/>
+      <c r="CW44" s="104"/>
+      <c r="CX44" s="104"/>
+      <c r="CY44" s="104"/>
+      <c r="CZ44" s="104"/>
+      <c r="DA44" s="104"/>
+      <c r="DB44" s="104"/>
+      <c r="DC44" s="104"/>
+      <c r="DD44" s="104"/>
+      <c r="DE44" s="104"/>
+      <c r="DF44" s="104"/>
+      <c r="DG44" s="104"/>
+      <c r="DH44" s="104"/>
+      <c r="DI44" s="104"/>
+      <c r="DJ44" s="104"/>
+      <c r="DK44" s="104"/>
+      <c r="DL44" s="104"/>
+      <c r="DM44" s="104"/>
+      <c r="DN44" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="DO42" s="106"/>
-      <c r="DP42" s="106"/>
-      <c r="DQ42" s="106"/>
-      <c r="DR42" s="106"/>
-      <c r="DS42" s="106"/>
-      <c r="DT42" s="106"/>
-      <c r="DU42" s="106"/>
-      <c r="DV42" s="106"/>
-      <c r="DW42" s="106"/>
-      <c r="DX42" s="106"/>
-      <c r="DY42" s="106"/>
-      <c r="DZ42" s="106"/>
-      <c r="EA42" s="106"/>
-      <c r="EB42" s="106"/>
-      <c r="EC42" s="107"/>
-      <c r="ED42" s="105" t="s">
+      <c r="DO44" s="106"/>
+      <c r="DP44" s="106"/>
+      <c r="DQ44" s="106"/>
+      <c r="DR44" s="106"/>
+      <c r="DS44" s="106"/>
+      <c r="DT44" s="106"/>
+      <c r="DU44" s="106"/>
+      <c r="DV44" s="106"/>
+      <c r="DW44" s="106"/>
+      <c r="DX44" s="106"/>
+      <c r="DY44" s="106"/>
+      <c r="DZ44" s="106"/>
+      <c r="EA44" s="106"/>
+      <c r="EB44" s="106"/>
+      <c r="EC44" s="107"/>
+      <c r="ED44" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="EE42" s="106"/>
-      <c r="EF42" s="106"/>
-      <c r="EG42" s="106"/>
-      <c r="EH42" s="106"/>
-      <c r="EI42" s="106"/>
-      <c r="EJ42" s="106"/>
-      <c r="EK42" s="106"/>
-      <c r="EL42" s="106"/>
-      <c r="EM42" s="106"/>
-      <c r="EN42" s="106"/>
-      <c r="EO42" s="106"/>
-      <c r="EP42" s="106"/>
-      <c r="EQ42" s="106"/>
-      <c r="ER42" s="106"/>
-      <c r="ES42" s="107"/>
-      <c r="ET42" s="74">
-        <v>1.2960000000000003</v>
-      </c>
-      <c r="EU42" s="75"/>
-      <c r="EV42" s="75"/>
-      <c r="EW42" s="75"/>
-      <c r="EX42" s="75"/>
-      <c r="EY42" s="75"/>
-      <c r="EZ42" s="75"/>
-      <c r="FA42" s="75"/>
-      <c r="FB42" s="75"/>
-      <c r="FC42" s="75"/>
-      <c r="FD42" s="75"/>
-      <c r="FE42" s="75"/>
-      <c r="FF42" s="75"/>
-      <c r="FG42" s="75"/>
-      <c r="FH42" s="75"/>
-      <c r="FI42" s="76"/>
+      <c r="EE44" s="106"/>
+      <c r="EF44" s="106"/>
+      <c r="EG44" s="106"/>
+      <c r="EH44" s="106"/>
+      <c r="EI44" s="106"/>
+      <c r="EJ44" s="106"/>
+      <c r="EK44" s="106"/>
+      <c r="EL44" s="106"/>
+      <c r="EM44" s="106"/>
+      <c r="EN44" s="106"/>
+      <c r="EO44" s="106"/>
+      <c r="EP44" s="106"/>
+      <c r="EQ44" s="106"/>
+      <c r="ER44" s="106"/>
+      <c r="ES44" s="107"/>
+      <c r="ET44" s="74">
+        <v>1.7280000000000002</v>
+      </c>
+      <c r="EU44" s="75"/>
+      <c r="EV44" s="75"/>
+      <c r="EW44" s="75"/>
+      <c r="EX44" s="75"/>
+      <c r="EY44" s="75"/>
+      <c r="EZ44" s="75"/>
+      <c r="FA44" s="75"/>
+      <c r="FB44" s="75"/>
+      <c r="FC44" s="75"/>
+      <c r="FD44" s="75"/>
+      <c r="FE44" s="75"/>
+      <c r="FF44" s="75"/>
+      <c r="FG44" s="75"/>
+      <c r="FH44" s="75"/>
+      <c r="FI44" s="76"/>
     </row>
-    <row r="43" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="A43" s="103"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="103"/>
-      <c r="D43" s="103"/>
-      <c r="E43" s="103"/>
-      <c r="F43" s="103"/>
-      <c r="G43" s="103"/>
-      <c r="H43" s="103"/>
-      <c r="I43" s="103"/>
-      <c r="J43" s="103"/>
-      <c r="K43" s="103"/>
-      <c r="L43" s="103"/>
-      <c r="M43" s="103"/>
-      <c r="N43" s="103"/>
-      <c r="O43" s="103"/>
-      <c r="P43" s="103"/>
-      <c r="Q43" s="103"/>
-      <c r="R43" s="103"/>
-      <c r="S43" s="103"/>
-      <c r="T43" s="103"/>
-      <c r="U43" s="103"/>
-      <c r="V43" s="103"/>
-      <c r="W43" s="103"/>
-      <c r="X43" s="103"/>
-      <c r="Y43" s="103"/>
-      <c r="Z43" s="103"/>
-      <c r="AA43" s="103"/>
-      <c r="AB43" s="103"/>
-      <c r="AC43" s="103"/>
-      <c r="AD43" s="103"/>
-      <c r="AE43" s="103"/>
-      <c r="AF43" s="103"/>
-      <c r="AG43" s="103"/>
-      <c r="AH43" s="103"/>
-      <c r="AI43" s="103"/>
-      <c r="AJ43" s="103"/>
-      <c r="AK43" s="103"/>
-      <c r="AL43" s="103"/>
-      <c r="AM43" s="103"/>
-      <c r="AN43" s="103"/>
-      <c r="AO43" s="103"/>
-      <c r="AP43" s="103"/>
-      <c r="AQ43" s="103"/>
-      <c r="AR43" s="103"/>
-      <c r="AS43" s="103"/>
-      <c r="AT43" s="103"/>
-      <c r="AU43" s="103"/>
-      <c r="AV43" s="103"/>
-      <c r="AW43" s="103"/>
-      <c r="AX43" s="103"/>
-      <c r="AY43" s="103"/>
-      <c r="AZ43" s="103"/>
-      <c r="BA43" s="103"/>
-      <c r="BB43" s="103"/>
-      <c r="BC43" s="103"/>
-      <c r="BD43" s="103"/>
-      <c r="BE43" s="103"/>
-      <c r="BF43" s="103"/>
-      <c r="BG43" s="103"/>
-      <c r="BH43" s="103"/>
-      <c r="BI43" s="103"/>
-      <c r="BJ43" s="103"/>
-      <c r="BK43" s="103"/>
-      <c r="BL43" s="103"/>
-      <c r="BM43" s="103"/>
-      <c r="BN43" s="103"/>
-      <c r="BO43" s="103"/>
-      <c r="BP43" s="103"/>
-      <c r="BQ43" s="103"/>
-      <c r="BR43" s="103"/>
-      <c r="BS43" s="103"/>
-      <c r="BT43" s="103"/>
-      <c r="BU43" s="103"/>
-      <c r="BV43" s="103"/>
-      <c r="BW43" s="103"/>
-      <c r="BX43" s="103"/>
-      <c r="BY43" s="103"/>
-      <c r="BZ43" s="103"/>
-      <c r="CA43" s="103"/>
-      <c r="CB43" s="103"/>
-      <c r="CC43" s="103"/>
-      <c r="CD43" s="103"/>
-      <c r="CE43" s="103"/>
-      <c r="CF43" s="103"/>
-      <c r="CG43" s="103"/>
-      <c r="CH43" s="103"/>
-      <c r="CI43" s="103"/>
-      <c r="CJ43" s="103"/>
-      <c r="CK43" s="103"/>
-      <c r="CL43" s="103"/>
-      <c r="CM43" s="103"/>
-      <c r="CN43" s="103"/>
-      <c r="CO43" s="103"/>
-      <c r="CP43" s="104" t="s">
+    <row r="45" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="A45" s="103"/>
+      <c r="B45" s="103"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="103"/>
+      <c r="E45" s="103"/>
+      <c r="F45" s="103"/>
+      <c r="G45" s="103"/>
+      <c r="H45" s="103"/>
+      <c r="I45" s="103"/>
+      <c r="J45" s="103"/>
+      <c r="K45" s="103"/>
+      <c r="L45" s="103"/>
+      <c r="M45" s="103"/>
+      <c r="N45" s="103"/>
+      <c r="O45" s="103"/>
+      <c r="P45" s="103"/>
+      <c r="Q45" s="103"/>
+      <c r="R45" s="103"/>
+      <c r="S45" s="103"/>
+      <c r="T45" s="103"/>
+      <c r="U45" s="103"/>
+      <c r="V45" s="103"/>
+      <c r="W45" s="103"/>
+      <c r="X45" s="103"/>
+      <c r="Y45" s="103"/>
+      <c r="Z45" s="103"/>
+      <c r="AA45" s="103"/>
+      <c r="AB45" s="103"/>
+      <c r="AC45" s="103"/>
+      <c r="AD45" s="103"/>
+      <c r="AE45" s="103"/>
+      <c r="AF45" s="103"/>
+      <c r="AG45" s="103"/>
+      <c r="AH45" s="103"/>
+      <c r="AI45" s="103"/>
+      <c r="AJ45" s="103"/>
+      <c r="AK45" s="103"/>
+      <c r="AL45" s="103"/>
+      <c r="AM45" s="103"/>
+      <c r="AN45" s="103"/>
+      <c r="AO45" s="103"/>
+      <c r="AP45" s="103"/>
+      <c r="AQ45" s="103"/>
+      <c r="AR45" s="103"/>
+      <c r="AS45" s="103"/>
+      <c r="AT45" s="103"/>
+      <c r="AU45" s="103"/>
+      <c r="AV45" s="103"/>
+      <c r="AW45" s="103"/>
+      <c r="AX45" s="103"/>
+      <c r="AY45" s="103"/>
+      <c r="AZ45" s="103"/>
+      <c r="BA45" s="103"/>
+      <c r="BB45" s="103"/>
+      <c r="BC45" s="103"/>
+      <c r="BD45" s="103"/>
+      <c r="BE45" s="103"/>
+      <c r="BF45" s="103"/>
+      <c r="BG45" s="103"/>
+      <c r="BH45" s="103"/>
+      <c r="BI45" s="103"/>
+      <c r="BJ45" s="103"/>
+      <c r="BK45" s="103"/>
+      <c r="BL45" s="103"/>
+      <c r="BM45" s="103"/>
+      <c r="BN45" s="103"/>
+      <c r="BO45" s="103"/>
+      <c r="BP45" s="103"/>
+      <c r="BQ45" s="103"/>
+      <c r="BR45" s="103"/>
+      <c r="BS45" s="103"/>
+      <c r="BT45" s="103"/>
+      <c r="BU45" s="103"/>
+      <c r="BV45" s="103"/>
+      <c r="BW45" s="103"/>
+      <c r="BX45" s="103"/>
+      <c r="BY45" s="103"/>
+      <c r="BZ45" s="103"/>
+      <c r="CA45" s="103"/>
+      <c r="CB45" s="103"/>
+      <c r="CC45" s="103"/>
+      <c r="CD45" s="103"/>
+      <c r="CE45" s="103"/>
+      <c r="CF45" s="103"/>
+      <c r="CG45" s="103"/>
+      <c r="CH45" s="103"/>
+      <c r="CI45" s="103"/>
+      <c r="CJ45" s="103"/>
+      <c r="CK45" s="103"/>
+      <c r="CL45" s="103"/>
+      <c r="CM45" s="103"/>
+      <c r="CN45" s="103"/>
+      <c r="CO45" s="103"/>
+      <c r="CP45" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="CQ43" s="104"/>
-      <c r="CR43" s="104"/>
-      <c r="CS43" s="104"/>
-      <c r="CT43" s="104"/>
-      <c r="CU43" s="104"/>
-      <c r="CV43" s="104"/>
-      <c r="CW43" s="104"/>
-      <c r="CX43" s="104"/>
-      <c r="CY43" s="104"/>
-      <c r="CZ43" s="104"/>
-      <c r="DA43" s="104"/>
-      <c r="DB43" s="104"/>
-      <c r="DC43" s="104"/>
-      <c r="DD43" s="104"/>
-      <c r="DE43" s="104"/>
-      <c r="DF43" s="104"/>
-      <c r="DG43" s="104"/>
-      <c r="DH43" s="104"/>
-      <c r="DI43" s="104"/>
-      <c r="DJ43" s="104"/>
-      <c r="DK43" s="104"/>
-      <c r="DL43" s="104"/>
-      <c r="DM43" s="104"/>
-      <c r="DN43" s="74" t="s">
-        <v>99</v>
-      </c>
-      <c r="DO43" s="75"/>
-      <c r="DP43" s="75"/>
-      <c r="DQ43" s="75"/>
-      <c r="DR43" s="75"/>
-      <c r="DS43" s="75"/>
-      <c r="DT43" s="75"/>
-      <c r="DU43" s="75"/>
-      <c r="DV43" s="75"/>
-      <c r="DW43" s="75"/>
-      <c r="DX43" s="75"/>
-      <c r="DY43" s="75"/>
-      <c r="DZ43" s="75"/>
-      <c r="EA43" s="75"/>
-      <c r="EB43" s="75"/>
-      <c r="EC43" s="76"/>
-      <c r="ED43" s="105" t="s">
+      <c r="CQ45" s="104"/>
+      <c r="CR45" s="104"/>
+      <c r="CS45" s="104"/>
+      <c r="CT45" s="104"/>
+      <c r="CU45" s="104"/>
+      <c r="CV45" s="104"/>
+      <c r="CW45" s="104"/>
+      <c r="CX45" s="104"/>
+      <c r="CY45" s="104"/>
+      <c r="CZ45" s="104"/>
+      <c r="DA45" s="104"/>
+      <c r="DB45" s="104"/>
+      <c r="DC45" s="104"/>
+      <c r="DD45" s="104"/>
+      <c r="DE45" s="104"/>
+      <c r="DF45" s="104"/>
+      <c r="DG45" s="104"/>
+      <c r="DH45" s="104"/>
+      <c r="DI45" s="104"/>
+      <c r="DJ45" s="104"/>
+      <c r="DK45" s="104"/>
+      <c r="DL45" s="104"/>
+      <c r="DM45" s="104"/>
+      <c r="DN45" s="74">
+        <v>10</v>
+      </c>
+      <c r="DO45" s="75"/>
+      <c r="DP45" s="75"/>
+      <c r="DQ45" s="75"/>
+      <c r="DR45" s="75"/>
+      <c r="DS45" s="75"/>
+      <c r="DT45" s="75"/>
+      <c r="DU45" s="75"/>
+      <c r="DV45" s="75"/>
+      <c r="DW45" s="75"/>
+      <c r="DX45" s="75"/>
+      <c r="DY45" s="75"/>
+      <c r="DZ45" s="75"/>
+      <c r="EA45" s="75"/>
+      <c r="EB45" s="75"/>
+      <c r="EC45" s="76"/>
+      <c r="ED45" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="EE43" s="106"/>
-      <c r="EF43" s="106"/>
-      <c r="EG43" s="106"/>
-      <c r="EH43" s="106"/>
-      <c r="EI43" s="106"/>
-      <c r="EJ43" s="106"/>
-      <c r="EK43" s="106"/>
-      <c r="EL43" s="106"/>
-      <c r="EM43" s="106"/>
-      <c r="EN43" s="106"/>
-      <c r="EO43" s="106"/>
-      <c r="EP43" s="106"/>
-      <c r="EQ43" s="106"/>
-      <c r="ER43" s="106"/>
-      <c r="ES43" s="107"/>
-      <c r="ET43" s="74">
-        <v>7.776000000000001</v>
-      </c>
-      <c r="EU43" s="75"/>
-      <c r="EV43" s="75"/>
-      <c r="EW43" s="75"/>
-      <c r="EX43" s="75"/>
-      <c r="EY43" s="75"/>
-      <c r="EZ43" s="75"/>
-      <c r="FA43" s="75"/>
-      <c r="FB43" s="75"/>
-      <c r="FC43" s="75"/>
-      <c r="FD43" s="75"/>
-      <c r="FE43" s="75"/>
-      <c r="FF43" s="75"/>
-      <c r="FG43" s="75"/>
-      <c r="FH43" s="75"/>
-      <c r="FI43" s="76"/>
+      <c r="EE45" s="106"/>
+      <c r="EF45" s="106"/>
+      <c r="EG45" s="106"/>
+      <c r="EH45" s="106"/>
+      <c r="EI45" s="106"/>
+      <c r="EJ45" s="106"/>
+      <c r="EK45" s="106"/>
+      <c r="EL45" s="106"/>
+      <c r="EM45" s="106"/>
+      <c r="EN45" s="106"/>
+      <c r="EO45" s="106"/>
+      <c r="EP45" s="106"/>
+      <c r="EQ45" s="106"/>
+      <c r="ER45" s="106"/>
+      <c r="ES45" s="107"/>
+      <c r="ET45" s="74">
+        <v>10.368</v>
+      </c>
+      <c r="EU45" s="75"/>
+      <c r="EV45" s="75"/>
+      <c r="EW45" s="75"/>
+      <c r="EX45" s="75"/>
+      <c r="EY45" s="75"/>
+      <c r="EZ45" s="75"/>
+      <c r="FA45" s="75"/>
+      <c r="FB45" s="75"/>
+      <c r="FC45" s="75"/>
+      <c r="FD45" s="75"/>
+      <c r="FE45" s="75"/>
+      <c r="FF45" s="75"/>
+      <c r="FG45" s="75"/>
+      <c r="FH45" s="75"/>
+      <c r="FI45" s="76"/>
     </row>
-    <row customHeight="1" ht="8.1" r="44" spans="1:702" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="I45" s="16" t="s">
+    <row customHeight="1" ht="8.1" r="46" spans="1:702" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="I47" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="J45" s="16"/>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16"/>
-      <c r="M45" s="16"/>
-      <c r="N45" s="16"/>
-      <c r="O45" s="16"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="67" t="s">
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
-      <c r="V45" s="18"/>
-      <c r="W45" s="18"/>
-      <c r="X45" s="18"/>
-      <c r="Y45" s="18"/>
-      <c r="Z45" s="18"/>
-      <c r="AA45" s="18"/>
-      <c r="AB45" s="18"/>
-      <c r="AC45" s="18"/>
-      <c r="AD45" s="18"/>
-      <c r="AE45" s="18"/>
-      <c r="AF45" s="18"/>
-      <c r="AG45" s="18"/>
-      <c r="AH45" s="18"/>
-      <c r="AI45" s="18"/>
-      <c r="AJ45" s="18"/>
-      <c r="AK45" s="18"/>
-      <c r="AL45" s="18"/>
-      <c r="AM45" s="18"/>
-      <c r="AN45" s="18"/>
-      <c r="AO45" s="18"/>
-      <c r="AP45" s="18"/>
-      <c r="AQ45" s="18"/>
-      <c r="AR45" s="18"/>
-      <c r="AS45" s="18"/>
-      <c r="AT45" s="18"/>
-      <c r="AU45" s="18"/>
-      <c r="AV45" s="18"/>
-      <c r="AW45" s="18"/>
-      <c r="AX45" s="18"/>
-      <c r="AY45" s="18"/>
-      <c r="AZ45" s="18"/>
-      <c r="BA45" s="18"/>
-      <c r="BC45" s="68"/>
-      <c r="BD45" s="68"/>
-      <c r="BE45" s="68"/>
-      <c r="BF45" s="68"/>
-      <c r="BG45" s="68"/>
-      <c r="BH45" s="68"/>
-      <c r="BI45" s="68"/>
-      <c r="BJ45" s="68"/>
-      <c r="BK45" s="68"/>
-      <c r="BL45" s="68"/>
-      <c r="BM45" s="68"/>
-      <c r="BN45" s="68"/>
-      <c r="BO45" s="68"/>
-      <c r="BP45" s="68"/>
-      <c r="BQ45" s="68"/>
-      <c r="BR45" s="68"/>
-      <c r="BS45" s="68"/>
-      <c r="BT45" s="68"/>
-      <c r="BU45" s="68"/>
-      <c r="BV45" s="68"/>
-      <c r="BW45" s="68"/>
-      <c r="BX45" s="68"/>
-      <c r="BY45" s="68"/>
-      <c r="BZ45" s="68"/>
-      <c r="CA45" s="68"/>
-      <c r="CB45" s="68"/>
-      <c r="CC45" s="68"/>
-      <c r="CD45" s="68"/>
-      <c r="CE45" s="68"/>
-      <c r="CF45" s="68"/>
-      <c r="CG45" s="68"/>
-      <c r="CH45" s="68"/>
-      <c r="CI45" s="68"/>
-      <c r="CK45" s="67" t="s">
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="18"/>
+      <c r="U47" s="18"/>
+      <c r="V47" s="18"/>
+      <c r="W47" s="18"/>
+      <c r="X47" s="18"/>
+      <c r="Y47" s="18"/>
+      <c r="Z47" s="18"/>
+      <c r="AA47" s="18"/>
+      <c r="AB47" s="18"/>
+      <c r="AC47" s="18"/>
+      <c r="AD47" s="18"/>
+      <c r="AE47" s="18"/>
+      <c r="AF47" s="18"/>
+      <c r="AG47" s="18"/>
+      <c r="AH47" s="18"/>
+      <c r="AI47" s="18"/>
+      <c r="AJ47" s="18"/>
+      <c r="AK47" s="18"/>
+      <c r="AL47" s="18"/>
+      <c r="AM47" s="18"/>
+      <c r="AN47" s="18"/>
+      <c r="AO47" s="18"/>
+      <c r="AP47" s="18"/>
+      <c r="AQ47" s="18"/>
+      <c r="AR47" s="18"/>
+      <c r="AS47" s="18"/>
+      <c r="AT47" s="18"/>
+      <c r="AU47" s="18"/>
+      <c r="AV47" s="18"/>
+      <c r="AW47" s="18"/>
+      <c r="AX47" s="18"/>
+      <c r="AY47" s="18"/>
+      <c r="AZ47" s="18"/>
+      <c r="BA47" s="18"/>
+      <c r="BC47" s="68"/>
+      <c r="BD47" s="68"/>
+      <c r="BE47" s="68"/>
+      <c r="BF47" s="68"/>
+      <c r="BG47" s="68"/>
+      <c r="BH47" s="68"/>
+      <c r="BI47" s="68"/>
+      <c r="BJ47" s="68"/>
+      <c r="BK47" s="68"/>
+      <c r="BL47" s="68"/>
+      <c r="BM47" s="68"/>
+      <c r="BN47" s="68"/>
+      <c r="BO47" s="68"/>
+      <c r="BP47" s="68"/>
+      <c r="BQ47" s="68"/>
+      <c r="BR47" s="68"/>
+      <c r="BS47" s="68"/>
+      <c r="BT47" s="68"/>
+      <c r="BU47" s="68"/>
+      <c r="BV47" s="68"/>
+      <c r="BW47" s="68"/>
+      <c r="BX47" s="68"/>
+      <c r="BY47" s="68"/>
+      <c r="BZ47" s="68"/>
+      <c r="CA47" s="68"/>
+      <c r="CB47" s="68"/>
+      <c r="CC47" s="68"/>
+      <c r="CD47" s="68"/>
+      <c r="CE47" s="68"/>
+      <c r="CF47" s="68"/>
+      <c r="CG47" s="68"/>
+      <c r="CH47" s="68"/>
+      <c r="CI47" s="68"/>
+      <c r="CK47" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="CL45" s="18"/>
-      <c r="CM45" s="18"/>
-      <c r="CN45" s="18"/>
-      <c r="CO45" s="18"/>
-      <c r="CP45" s="18"/>
-      <c r="CQ45" s="18"/>
-      <c r="CR45" s="18"/>
-      <c r="CS45" s="18"/>
-      <c r="CT45" s="18"/>
-      <c r="CU45" s="18"/>
-      <c r="CV45" s="18"/>
-      <c r="CW45" s="18"/>
-      <c r="CX45" s="18"/>
-      <c r="CY45" s="18"/>
-      <c r="CZ45" s="18"/>
-      <c r="DA45" s="18"/>
-      <c r="DB45" s="18"/>
-      <c r="DC45" s="18"/>
-      <c r="DD45" s="18"/>
-      <c r="DE45" s="18"/>
-      <c r="DF45" s="18"/>
-      <c r="DG45" s="18"/>
-      <c r="DH45" s="18"/>
-      <c r="DI45" s="18"/>
-      <c r="DJ45" s="18"/>
-      <c r="DK45" s="18"/>
-      <c r="DL45" s="18"/>
-      <c r="DM45" s="18"/>
-      <c r="DN45" s="18"/>
-      <c r="DO45" s="18"/>
-      <c r="DP45" s="18"/>
-      <c r="DQ45" s="18"/>
-      <c r="DR45" s="18"/>
-      <c r="DS45" s="18"/>
-      <c r="DT45" s="18"/>
-      <c r="DU45" s="18"/>
-      <c r="DV45" s="18"/>
-      <c r="DW45" s="18"/>
-      <c r="DX45" s="18"/>
-      <c r="DY45" s="18"/>
-      <c r="DZ45" s="18"/>
-      <c r="EA45" s="18"/>
-      <c r="EB45" s="18"/>
-      <c r="EC45" s="18"/>
-      <c r="ED45" s="18"/>
-      <c r="EE45" s="18"/>
-      <c r="EF45" s="18"/>
-      <c r="EG45" s="18"/>
-      <c r="EH45" s="18"/>
-      <c r="EI45" s="18"/>
-      <c r="EJ45" s="18"/>
-      <c r="EK45" s="18"/>
-      <c r="EL45" s="18"/>
-      <c r="EM45" s="18"/>
-      <c r="EN45" s="18"/>
-      <c r="EO45" s="18"/>
-      <c r="EP45" s="18"/>
-      <c r="EQ45" s="18"/>
-      <c r="ER45" s="18"/>
-      <c r="ES45" s="18"/>
-      <c r="ET45" s="18"/>
-      <c r="EU45" s="18"/>
-      <c r="EV45" s="18"/>
-      <c r="EW45" s="18"/>
-      <c r="EX45" s="18"/>
-      <c r="EY45" s="18"/>
-      <c r="EZ45" s="18"/>
-      <c r="FA45" s="18"/>
-      <c r="FB45" s="18"/>
-      <c r="FC45" s="18"/>
-      <c r="FD45" s="18"/>
-      <c r="FE45" s="18"/>
-      <c r="FF45" s="18"/>
-      <c r="FG45" s="18"/>
-      <c r="FH45" s="18"/>
-      <c r="FI45" s="18"/>
+      <c r="CL47" s="18"/>
+      <c r="CM47" s="18"/>
+      <c r="CN47" s="18"/>
+      <c r="CO47" s="18"/>
+      <c r="CP47" s="18"/>
+      <c r="CQ47" s="18"/>
+      <c r="CR47" s="18"/>
+      <c r="CS47" s="18"/>
+      <c r="CT47" s="18"/>
+      <c r="CU47" s="18"/>
+      <c r="CV47" s="18"/>
+      <c r="CW47" s="18"/>
+      <c r="CX47" s="18"/>
+      <c r="CY47" s="18"/>
+      <c r="CZ47" s="18"/>
+      <c r="DA47" s="18"/>
+      <c r="DB47" s="18"/>
+      <c r="DC47" s="18"/>
+      <c r="DD47" s="18"/>
+      <c r="DE47" s="18"/>
+      <c r="DF47" s="18"/>
+      <c r="DG47" s="18"/>
+      <c r="DH47" s="18"/>
+      <c r="DI47" s="18"/>
+      <c r="DJ47" s="18"/>
+      <c r="DK47" s="18"/>
+      <c r="DL47" s="18"/>
+      <c r="DM47" s="18"/>
+      <c r="DN47" s="18"/>
+      <c r="DO47" s="18"/>
+      <c r="DP47" s="18"/>
+      <c r="DQ47" s="18"/>
+      <c r="DR47" s="18"/>
+      <c r="DS47" s="18"/>
+      <c r="DT47" s="18"/>
+      <c r="DU47" s="18"/>
+      <c r="DV47" s="18"/>
+      <c r="DW47" s="18"/>
+      <c r="DX47" s="18"/>
+      <c r="DY47" s="18"/>
+      <c r="DZ47" s="18"/>
+      <c r="EA47" s="18"/>
+      <c r="EB47" s="18"/>
+      <c r="EC47" s="18"/>
+      <c r="ED47" s="18"/>
+      <c r="EE47" s="18"/>
+      <c r="EF47" s="18"/>
+      <c r="EG47" s="18"/>
+      <c r="EH47" s="18"/>
+      <c r="EI47" s="18"/>
+      <c r="EJ47" s="18"/>
+      <c r="EK47" s="18"/>
+      <c r="EL47" s="18"/>
+      <c r="EM47" s="18"/>
+      <c r="EN47" s="18"/>
+      <c r="EO47" s="18"/>
+      <c r="EP47" s="18"/>
+      <c r="EQ47" s="18"/>
+      <c r="ER47" s="18"/>
+      <c r="ES47" s="18"/>
+      <c r="ET47" s="18"/>
+      <c r="EU47" s="18"/>
+      <c r="EV47" s="18"/>
+      <c r="EW47" s="18"/>
+      <c r="EX47" s="18"/>
+      <c r="EY47" s="18"/>
+      <c r="EZ47" s="18"/>
+      <c r="FA47" s="18"/>
+      <c r="FB47" s="18"/>
+      <c r="FC47" s="18"/>
+      <c r="FD47" s="18"/>
+      <c r="FE47" s="18"/>
+      <c r="FF47" s="18"/>
+      <c r="FG47" s="18"/>
+      <c r="FH47" s="18"/>
+      <c r="FI47" s="18"/>
     </row>
-    <row customHeight="1" ht="6.9" r="46" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="Q46" s="3" t="s">
+    <row customHeight="1" ht="6.9" r="48" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="Q48" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
-      <c r="AA46" s="3"/>
-      <c r="AB46" s="3"/>
-      <c r="AC46" s="3"/>
-      <c r="AD46" s="3"/>
-      <c r="AE46" s="3"/>
-      <c r="AF46" s="3"/>
-      <c r="AG46" s="3"/>
-      <c r="AH46" s="3"/>
-      <c r="AI46" s="3"/>
-      <c r="AJ46" s="3"/>
-      <c r="AK46" s="3"/>
-      <c r="AL46" s="3"/>
-      <c r="AM46" s="3"/>
-      <c r="AN46" s="3"/>
-      <c r="AO46" s="3"/>
-      <c r="AP46" s="3"/>
-      <c r="AQ46" s="3"/>
-      <c r="AR46" s="3"/>
-      <c r="AS46" s="3"/>
-      <c r="AT46" s="3"/>
-      <c r="AU46" s="3"/>
-      <c r="AV46" s="3"/>
-      <c r="AW46" s="3"/>
-      <c r="AX46" s="3"/>
-      <c r="AY46" s="3"/>
-      <c r="AZ46" s="3"/>
-      <c r="BA46" s="3"/>
-      <c r="BC46" s="3" t="s">
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3"/>
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="3"/>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+      <c r="AJ48" s="3"/>
+      <c r="AK48" s="3"/>
+      <c r="AL48" s="3"/>
+      <c r="AM48" s="3"/>
+      <c r="AN48" s="3"/>
+      <c r="AO48" s="3"/>
+      <c r="AP48" s="3"/>
+      <c r="AQ48" s="3"/>
+      <c r="AR48" s="3"/>
+      <c r="AS48" s="3"/>
+      <c r="AT48" s="3"/>
+      <c r="AU48" s="3"/>
+      <c r="AV48" s="3"/>
+      <c r="AW48" s="3"/>
+      <c r="AX48" s="3"/>
+      <c r="AY48" s="3"/>
+      <c r="AZ48" s="3"/>
+      <c r="BA48" s="3"/>
+      <c r="BC48" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BD46" s="3"/>
-      <c r="BE46" s="3"/>
-      <c r="BF46" s="3"/>
-      <c r="BG46" s="3"/>
-      <c r="BH46" s="3"/>
-      <c r="BI46" s="3"/>
-      <c r="BJ46" s="3"/>
-      <c r="BK46" s="3"/>
-      <c r="BL46" s="3"/>
-      <c r="BM46" s="3"/>
-      <c r="BN46" s="3"/>
-      <c r="BO46" s="3"/>
-      <c r="BP46" s="3"/>
-      <c r="BQ46" s="3"/>
-      <c r="BR46" s="3"/>
-      <c r="BS46" s="3"/>
-      <c r="BT46" s="3"/>
-      <c r="BU46" s="3"/>
-      <c r="BV46" s="3"/>
-      <c r="BW46" s="3"/>
-      <c r="BX46" s="3"/>
-      <c r="BY46" s="3"/>
-      <c r="BZ46" s="3"/>
-      <c r="CA46" s="3"/>
-      <c r="CB46" s="3"/>
-      <c r="CC46" s="3"/>
-      <c r="CD46" s="3"/>
-      <c r="CE46" s="3"/>
-      <c r="CF46" s="3"/>
-      <c r="CG46" s="3"/>
-      <c r="CH46" s="3"/>
-      <c r="CI46" s="3"/>
-      <c r="CK46" s="3" t="s">
+      <c r="BD48" s="3"/>
+      <c r="BE48" s="3"/>
+      <c r="BF48" s="3"/>
+      <c r="BG48" s="3"/>
+      <c r="BH48" s="3"/>
+      <c r="BI48" s="3"/>
+      <c r="BJ48" s="3"/>
+      <c r="BK48" s="3"/>
+      <c r="BL48" s="3"/>
+      <c r="BM48" s="3"/>
+      <c r="BN48" s="3"/>
+      <c r="BO48" s="3"/>
+      <c r="BP48" s="3"/>
+      <c r="BQ48" s="3"/>
+      <c r="BR48" s="3"/>
+      <c r="BS48" s="3"/>
+      <c r="BT48" s="3"/>
+      <c r="BU48" s="3"/>
+      <c r="BV48" s="3"/>
+      <c r="BW48" s="3"/>
+      <c r="BX48" s="3"/>
+      <c r="BY48" s="3"/>
+      <c r="BZ48" s="3"/>
+      <c r="CA48" s="3"/>
+      <c r="CB48" s="3"/>
+      <c r="CC48" s="3"/>
+      <c r="CD48" s="3"/>
+      <c r="CE48" s="3"/>
+      <c r="CF48" s="3"/>
+      <c r="CG48" s="3"/>
+      <c r="CH48" s="3"/>
+      <c r="CI48" s="3"/>
+      <c r="CK48" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="CL46" s="3"/>
-      <c r="CM46" s="3"/>
-      <c r="CN46" s="3"/>
-      <c r="CO46" s="3"/>
-      <c r="CP46" s="3"/>
-      <c r="CQ46" s="3"/>
-      <c r="CR46" s="3"/>
-      <c r="CS46" s="3"/>
-      <c r="CT46" s="3"/>
-      <c r="CU46" s="3"/>
-      <c r="CV46" s="3"/>
-      <c r="CW46" s="3"/>
-      <c r="CX46" s="3"/>
-      <c r="CY46" s="3"/>
-      <c r="CZ46" s="3"/>
-      <c r="DA46" s="3"/>
-      <c r="DB46" s="3"/>
-      <c r="DC46" s="3"/>
-      <c r="DD46" s="3"/>
-      <c r="DE46" s="3"/>
-      <c r="DF46" s="3"/>
-      <c r="DG46" s="3"/>
-      <c r="DH46" s="3"/>
-      <c r="DI46" s="3"/>
-      <c r="DJ46" s="3"/>
-      <c r="DK46" s="3"/>
-      <c r="DL46" s="3"/>
-      <c r="DM46" s="3"/>
-      <c r="DN46" s="3"/>
-      <c r="DO46" s="3"/>
-      <c r="DP46" s="3"/>
-      <c r="DQ46" s="3"/>
-      <c r="DR46" s="3"/>
-      <c r="DS46" s="3"/>
-      <c r="DT46" s="3"/>
-      <c r="DU46" s="3"/>
-      <c r="DV46" s="3"/>
-      <c r="DW46" s="3"/>
-      <c r="DX46" s="3"/>
-      <c r="DY46" s="3"/>
-      <c r="DZ46" s="3"/>
-      <c r="EA46" s="3"/>
-      <c r="EB46" s="3"/>
-      <c r="EC46" s="3"/>
-      <c r="ED46" s="3"/>
-      <c r="EE46" s="3"/>
-      <c r="EF46" s="3"/>
-      <c r="EG46" s="3"/>
-      <c r="EH46" s="3"/>
-      <c r="EI46" s="3"/>
-      <c r="EJ46" s="3"/>
-      <c r="EK46" s="3"/>
-      <c r="EL46" s="3"/>
-      <c r="EM46" s="3"/>
-      <c r="EN46" s="3"/>
-      <c r="EO46" s="3"/>
-      <c r="EP46" s="3"/>
-      <c r="EQ46" s="3"/>
-      <c r="ER46" s="3"/>
-      <c r="ES46" s="3"/>
-      <c r="ET46" s="3"/>
-      <c r="EU46" s="3"/>
-      <c r="EV46" s="3"/>
-      <c r="EW46" s="3"/>
-      <c r="EX46" s="3"/>
-      <c r="EY46" s="3"/>
-      <c r="EZ46" s="3"/>
-      <c r="FA46" s="3"/>
-      <c r="FB46" s="3"/>
-      <c r="FC46" s="3"/>
-      <c r="FD46" s="3"/>
-      <c r="FE46" s="3"/>
-      <c r="FF46" s="3"/>
-      <c r="FG46" s="3"/>
-      <c r="FH46" s="3"/>
-      <c r="FI46" s="3"/>
+      <c r="CL48" s="3"/>
+      <c r="CM48" s="3"/>
+      <c r="CN48" s="3"/>
+      <c r="CO48" s="3"/>
+      <c r="CP48" s="3"/>
+      <c r="CQ48" s="3"/>
+      <c r="CR48" s="3"/>
+      <c r="CS48" s="3"/>
+      <c r="CT48" s="3"/>
+      <c r="CU48" s="3"/>
+      <c r="CV48" s="3"/>
+      <c r="CW48" s="3"/>
+      <c r="CX48" s="3"/>
+      <c r="CY48" s="3"/>
+      <c r="CZ48" s="3"/>
+      <c r="DA48" s="3"/>
+      <c r="DB48" s="3"/>
+      <c r="DC48" s="3"/>
+      <c r="DD48" s="3"/>
+      <c r="DE48" s="3"/>
+      <c r="DF48" s="3"/>
+      <c r="DG48" s="3"/>
+      <c r="DH48" s="3"/>
+      <c r="DI48" s="3"/>
+      <c r="DJ48" s="3"/>
+      <c r="DK48" s="3"/>
+      <c r="DL48" s="3"/>
+      <c r="DM48" s="3"/>
+      <c r="DN48" s="3"/>
+      <c r="DO48" s="3"/>
+      <c r="DP48" s="3"/>
+      <c r="DQ48" s="3"/>
+      <c r="DR48" s="3"/>
+      <c r="DS48" s="3"/>
+      <c r="DT48" s="3"/>
+      <c r="DU48" s="3"/>
+      <c r="DV48" s="3"/>
+      <c r="DW48" s="3"/>
+      <c r="DX48" s="3"/>
+      <c r="DY48" s="3"/>
+      <c r="DZ48" s="3"/>
+      <c r="EA48" s="3"/>
+      <c r="EB48" s="3"/>
+      <c r="EC48" s="3"/>
+      <c r="ED48" s="3"/>
+      <c r="EE48" s="3"/>
+      <c r="EF48" s="3"/>
+      <c r="EG48" s="3"/>
+      <c r="EH48" s="3"/>
+      <c r="EI48" s="3"/>
+      <c r="EJ48" s="3"/>
+      <c r="EK48" s="3"/>
+      <c r="EL48" s="3"/>
+      <c r="EM48" s="3"/>
+      <c r="EN48" s="3"/>
+      <c r="EO48" s="3"/>
+      <c r="EP48" s="3"/>
+      <c r="EQ48" s="3"/>
+      <c r="ER48" s="3"/>
+      <c r="ES48" s="3"/>
+      <c r="ET48" s="3"/>
+      <c r="EU48" s="3"/>
+      <c r="EV48" s="3"/>
+      <c r="EW48" s="3"/>
+      <c r="EX48" s="3"/>
+      <c r="EY48" s="3"/>
+      <c r="EZ48" s="3"/>
+      <c r="FA48" s="3"/>
+      <c r="FB48" s="3"/>
+      <c r="FC48" s="3"/>
+      <c r="FD48" s="3"/>
+      <c r="FE48" s="3"/>
+      <c r="FF48" s="3"/>
+      <c r="FG48" s="3"/>
+      <c r="FH48" s="3"/>
+      <c r="FI48" s="3"/>
     </row>
-    <row r="47" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="U47" s="64" t="s">
+    <row r="49" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="U49" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="V47" s="64"/>
-      <c r="W47" s="64"/>
-      <c r="X47" s="64"/>
-      <c r="Y47" s="64"/>
-      <c r="Z47" s="64"/>
+      <c r="V49" s="64"/>
+      <c r="W49" s="64"/>
+      <c r="X49" s="64"/>
+      <c r="Y49" s="64"/>
+      <c r="Z49" s="64"/>
     </row>
-    <row customHeight="1" ht="6.9" r="48" spans="1:702" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="I49" s="16" t="s">
+    <row customHeight="1" ht="6.9" r="50" spans="1:702" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="I51" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="16"/>
-      <c r="M49" s="16"/>
-      <c r="N49" s="16"/>
-      <c r="O49" s="16"/>
-      <c r="P49" s="16"/>
-      <c r="Q49" s="108" t="s">
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="R49" s="109"/>
-      <c r="S49" s="109"/>
-      <c r="T49" s="109"/>
-      <c r="U49" s="109"/>
-      <c r="V49" s="109"/>
-      <c r="W49" s="109"/>
-      <c r="X49" s="109"/>
-      <c r="Y49" s="109"/>
-      <c r="Z49" s="109"/>
-      <c r="AA49" s="109"/>
-      <c r="AB49" s="109"/>
-      <c r="AC49" s="109"/>
-      <c r="AD49" s="109"/>
-      <c r="AE49" s="109"/>
-      <c r="AF49" s="109"/>
-      <c r="AG49" s="109"/>
-      <c r="AH49" s="109"/>
-      <c r="AI49" s="109"/>
-      <c r="AJ49" s="109"/>
-      <c r="AK49" s="109"/>
-      <c r="AL49" s="109"/>
-      <c r="AM49" s="109"/>
-      <c r="AN49" s="109"/>
-      <c r="AO49" s="109"/>
-      <c r="AP49" s="109"/>
-      <c r="AQ49" s="109"/>
-      <c r="AR49" s="109"/>
-      <c r="AS49" s="109"/>
-      <c r="AT49" s="109"/>
-      <c r="AU49" s="109"/>
-      <c r="AV49" s="109"/>
-      <c r="AW49" s="109"/>
-      <c r="AX49" s="109"/>
-      <c r="AY49" s="109"/>
-      <c r="AZ49" s="109"/>
-      <c r="BA49" s="109"/>
-      <c r="BB49" s="2"/>
-      <c r="BC49" s="66"/>
-      <c r="BD49" s="66"/>
-      <c r="BE49" s="66"/>
-      <c r="BF49" s="66"/>
-      <c r="BG49" s="66"/>
-      <c r="BH49" s="66"/>
-      <c r="BI49" s="66"/>
-      <c r="BJ49" s="66"/>
-      <c r="BK49" s="66"/>
-      <c r="BL49" s="66"/>
-      <c r="BM49" s="66"/>
-      <c r="BN49" s="66"/>
-      <c r="BO49" s="66"/>
-      <c r="BP49" s="66"/>
-      <c r="BQ49" s="66"/>
-      <c r="BR49" s="66"/>
-      <c r="BS49" s="66"/>
-      <c r="BT49" s="66"/>
-      <c r="BU49" s="66"/>
-      <c r="BV49" s="66"/>
-      <c r="BW49" s="66"/>
-      <c r="BX49" s="66"/>
-      <c r="BY49" s="66"/>
-      <c r="BZ49" s="66"/>
-      <c r="CA49" s="66"/>
-      <c r="CB49" s="66"/>
-      <c r="CC49" s="66"/>
-      <c r="CD49" s="66"/>
-      <c r="CE49" s="66"/>
-      <c r="CF49" s="66"/>
-      <c r="CG49" s="66"/>
-      <c r="CH49" s="66"/>
-      <c r="CI49" s="66"/>
-      <c r="CJ49" s="2"/>
-      <c r="CK49" s="108" t="s">
+      <c r="R51" s="109"/>
+      <c r="S51" s="109"/>
+      <c r="T51" s="109"/>
+      <c r="U51" s="109"/>
+      <c r="V51" s="109"/>
+      <c r="W51" s="109"/>
+      <c r="X51" s="109"/>
+      <c r="Y51" s="109"/>
+      <c r="Z51" s="109"/>
+      <c r="AA51" s="109"/>
+      <c r="AB51" s="109"/>
+      <c r="AC51" s="109"/>
+      <c r="AD51" s="109"/>
+      <c r="AE51" s="109"/>
+      <c r="AF51" s="109"/>
+      <c r="AG51" s="109"/>
+      <c r="AH51" s="109"/>
+      <c r="AI51" s="109"/>
+      <c r="AJ51" s="109"/>
+      <c r="AK51" s="109"/>
+      <c r="AL51" s="109"/>
+      <c r="AM51" s="109"/>
+      <c r="AN51" s="109"/>
+      <c r="AO51" s="109"/>
+      <c r="AP51" s="109"/>
+      <c r="AQ51" s="109"/>
+      <c r="AR51" s="109"/>
+      <c r="AS51" s="109"/>
+      <c r="AT51" s="109"/>
+      <c r="AU51" s="109"/>
+      <c r="AV51" s="109"/>
+      <c r="AW51" s="109"/>
+      <c r="AX51" s="109"/>
+      <c r="AY51" s="109"/>
+      <c r="AZ51" s="109"/>
+      <c r="BA51" s="109"/>
+      <c r="BB51" s="2"/>
+      <c r="BC51" s="66"/>
+      <c r="BD51" s="66"/>
+      <c r="BE51" s="66"/>
+      <c r="BF51" s="66"/>
+      <c r="BG51" s="66"/>
+      <c r="BH51" s="66"/>
+      <c r="BI51" s="66"/>
+      <c r="BJ51" s="66"/>
+      <c r="BK51" s="66"/>
+      <c r="BL51" s="66"/>
+      <c r="BM51" s="66"/>
+      <c r="BN51" s="66"/>
+      <c r="BO51" s="66"/>
+      <c r="BP51" s="66"/>
+      <c r="BQ51" s="66"/>
+      <c r="BR51" s="66"/>
+      <c r="BS51" s="66"/>
+      <c r="BT51" s="66"/>
+      <c r="BU51" s="66"/>
+      <c r="BV51" s="66"/>
+      <c r="BW51" s="66"/>
+      <c r="BX51" s="66"/>
+      <c r="BY51" s="66"/>
+      <c r="BZ51" s="66"/>
+      <c r="CA51" s="66"/>
+      <c r="CB51" s="66"/>
+      <c r="CC51" s="66"/>
+      <c r="CD51" s="66"/>
+      <c r="CE51" s="66"/>
+      <c r="CF51" s="66"/>
+      <c r="CG51" s="66"/>
+      <c r="CH51" s="66"/>
+      <c r="CI51" s="66"/>
+      <c r="CJ51" s="2"/>
+      <c r="CK51" s="108" t="s">
         <v>101</v>
       </c>
-      <c r="CL49" s="109"/>
-      <c r="CM49" s="109"/>
-      <c r="CN49" s="109"/>
-      <c r="CO49" s="109"/>
-      <c r="CP49" s="109"/>
-      <c r="CQ49" s="109"/>
-      <c r="CR49" s="109"/>
-      <c r="CS49" s="109"/>
-      <c r="CT49" s="109"/>
-      <c r="CU49" s="109"/>
-      <c r="CV49" s="109"/>
-      <c r="CW49" s="109"/>
-      <c r="CX49" s="109"/>
-      <c r="CY49" s="109"/>
-      <c r="CZ49" s="109"/>
-      <c r="DA49" s="109"/>
-      <c r="DB49" s="109"/>
-      <c r="DC49" s="109"/>
-      <c r="DD49" s="109"/>
-      <c r="DE49" s="109"/>
-      <c r="DF49" s="109"/>
-      <c r="DG49" s="109"/>
-      <c r="DH49" s="109"/>
-      <c r="DI49" s="109"/>
-      <c r="DJ49" s="109"/>
-      <c r="DK49" s="109"/>
-      <c r="DL49" s="109"/>
-      <c r="DM49" s="109"/>
-      <c r="DN49" s="109"/>
-      <c r="DO49" s="109"/>
-      <c r="DP49" s="109"/>
-      <c r="DQ49" s="109"/>
-      <c r="DR49" s="109"/>
-      <c r="DS49" s="109"/>
-      <c r="DT49" s="109"/>
-      <c r="DU49" s="109"/>
-      <c r="DV49" s="109"/>
-      <c r="DW49" s="109"/>
-      <c r="DX49" s="109"/>
-      <c r="DY49" s="109"/>
-      <c r="DZ49" s="109"/>
-      <c r="EA49" s="109"/>
-      <c r="EB49" s="109"/>
-      <c r="EC49" s="109"/>
-      <c r="ED49" s="109"/>
-      <c r="EE49" s="109"/>
-      <c r="EF49" s="109"/>
-      <c r="EG49" s="109"/>
-      <c r="EH49" s="109"/>
-      <c r="EI49" s="109"/>
-      <c r="EJ49" s="109"/>
-      <c r="EK49" s="109"/>
-      <c r="EL49" s="109"/>
-      <c r="EM49" s="109"/>
-      <c r="EN49" s="109"/>
-      <c r="EO49" s="109"/>
-      <c r="EP49" s="109"/>
-      <c r="EQ49" s="109"/>
-      <c r="ER49" s="109"/>
-      <c r="ES49" s="109"/>
-      <c r="ET49" s="109"/>
-      <c r="EU49" s="109"/>
-      <c r="EV49" s="109"/>
-      <c r="EW49" s="109"/>
-      <c r="EX49" s="109"/>
-      <c r="EY49" s="109"/>
-      <c r="EZ49" s="109"/>
-      <c r="FA49" s="109"/>
-      <c r="FB49" s="109"/>
-      <c r="FC49" s="109"/>
-      <c r="FD49" s="109"/>
-      <c r="FE49" s="109"/>
-      <c r="FF49" s="109"/>
-      <c r="FG49" s="109"/>
-      <c r="FH49" s="109"/>
-      <c r="FI49" s="109"/>
+      <c r="CL51" s="109"/>
+      <c r="CM51" s="109"/>
+      <c r="CN51" s="109"/>
+      <c r="CO51" s="109"/>
+      <c r="CP51" s="109"/>
+      <c r="CQ51" s="109"/>
+      <c r="CR51" s="109"/>
+      <c r="CS51" s="109"/>
+      <c r="CT51" s="109"/>
+      <c r="CU51" s="109"/>
+      <c r="CV51" s="109"/>
+      <c r="CW51" s="109"/>
+      <c r="CX51" s="109"/>
+      <c r="CY51" s="109"/>
+      <c r="CZ51" s="109"/>
+      <c r="DA51" s="109"/>
+      <c r="DB51" s="109"/>
+      <c r="DC51" s="109"/>
+      <c r="DD51" s="109"/>
+      <c r="DE51" s="109"/>
+      <c r="DF51" s="109"/>
+      <c r="DG51" s="109"/>
+      <c r="DH51" s="109"/>
+      <c r="DI51" s="109"/>
+      <c r="DJ51" s="109"/>
+      <c r="DK51" s="109"/>
+      <c r="DL51" s="109"/>
+      <c r="DM51" s="109"/>
+      <c r="DN51" s="109"/>
+      <c r="DO51" s="109"/>
+      <c r="DP51" s="109"/>
+      <c r="DQ51" s="109"/>
+      <c r="DR51" s="109"/>
+      <c r="DS51" s="109"/>
+      <c r="DT51" s="109"/>
+      <c r="DU51" s="109"/>
+      <c r="DV51" s="109"/>
+      <c r="DW51" s="109"/>
+      <c r="DX51" s="109"/>
+      <c r="DY51" s="109"/>
+      <c r="DZ51" s="109"/>
+      <c r="EA51" s="109"/>
+      <c r="EB51" s="109"/>
+      <c r="EC51" s="109"/>
+      <c r="ED51" s="109"/>
+      <c r="EE51" s="109"/>
+      <c r="EF51" s="109"/>
+      <c r="EG51" s="109"/>
+      <c r="EH51" s="109"/>
+      <c r="EI51" s="109"/>
+      <c r="EJ51" s="109"/>
+      <c r="EK51" s="109"/>
+      <c r="EL51" s="109"/>
+      <c r="EM51" s="109"/>
+      <c r="EN51" s="109"/>
+      <c r="EO51" s="109"/>
+      <c r="EP51" s="109"/>
+      <c r="EQ51" s="109"/>
+      <c r="ER51" s="109"/>
+      <c r="ES51" s="109"/>
+      <c r="ET51" s="109"/>
+      <c r="EU51" s="109"/>
+      <c r="EV51" s="109"/>
+      <c r="EW51" s="109"/>
+      <c r="EX51" s="109"/>
+      <c r="EY51" s="109"/>
+      <c r="EZ51" s="109"/>
+      <c r="FA51" s="109"/>
+      <c r="FB51" s="109"/>
+      <c r="FC51" s="109"/>
+      <c r="FD51" s="109"/>
+      <c r="FE51" s="109"/>
+      <c r="FF51" s="109"/>
+      <c r="FG51" s="109"/>
+      <c r="FH51" s="109"/>
+      <c r="FI51" s="109"/>
     </row>
-    <row customHeight="1" ht="6.9" r="50" spans="1:702" x14ac:dyDescent="0.2">
-      <c r="Q50" s="3" t="s">
+    <row customHeight="1" ht="6.9" r="52" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="Q52" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-      <c r="V50" s="3"/>
-      <c r="W50" s="3"/>
-      <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
-      <c r="Z50" s="3"/>
-      <c r="AA50" s="3"/>
-      <c r="AB50" s="3"/>
-      <c r="AC50" s="3"/>
-      <c r="AD50" s="3"/>
-      <c r="AE50" s="3"/>
-      <c r="AF50" s="3"/>
-      <c r="AG50" s="3"/>
-      <c r="AH50" s="3"/>
-      <c r="AI50" s="3"/>
-      <c r="AJ50" s="3"/>
-      <c r="AK50" s="3"/>
-      <c r="AL50" s="3"/>
-      <c r="AM50" s="3"/>
-      <c r="AN50" s="3"/>
-      <c r="AO50" s="3"/>
-      <c r="AP50" s="3"/>
-      <c r="AQ50" s="3"/>
-      <c r="AR50" s="3"/>
-      <c r="AS50" s="3"/>
-      <c r="AT50" s="3"/>
-      <c r="AU50" s="3"/>
-      <c r="AV50" s="3"/>
-      <c r="AW50" s="3"/>
-      <c r="AX50" s="3"/>
-      <c r="AY50" s="3"/>
-      <c r="AZ50" s="3"/>
-      <c r="BA50" s="3"/>
-      <c r="BC50" s="3" t="s">
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
+      <c r="X52" s="3"/>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3"/>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="3"/>
+      <c r="AC52" s="3"/>
+      <c r="AD52" s="3"/>
+      <c r="AE52" s="3"/>
+      <c r="AF52" s="3"/>
+      <c r="AG52" s="3"/>
+      <c r="AH52" s="3"/>
+      <c r="AI52" s="3"/>
+      <c r="AJ52" s="3"/>
+      <c r="AK52" s="3"/>
+      <c r="AL52" s="3"/>
+      <c r="AM52" s="3"/>
+      <c r="AN52" s="3"/>
+      <c r="AO52" s="3"/>
+      <c r="AP52" s="3"/>
+      <c r="AQ52" s="3"/>
+      <c r="AR52" s="3"/>
+      <c r="AS52" s="3"/>
+      <c r="AT52" s="3"/>
+      <c r="AU52" s="3"/>
+      <c r="AV52" s="3"/>
+      <c r="AW52" s="3"/>
+      <c r="AX52" s="3"/>
+      <c r="AY52" s="3"/>
+      <c r="AZ52" s="3"/>
+      <c r="BA52" s="3"/>
+      <c r="BC52" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BD50" s="3"/>
-      <c r="BE50" s="3"/>
-      <c r="BF50" s="3"/>
-      <c r="BG50" s="3"/>
-      <c r="BH50" s="3"/>
-      <c r="BI50" s="3"/>
-      <c r="BJ50" s="3"/>
-      <c r="BK50" s="3"/>
-      <c r="BL50" s="3"/>
-      <c r="BM50" s="3"/>
-      <c r="BN50" s="3"/>
-      <c r="BO50" s="3"/>
-      <c r="BP50" s="3"/>
-      <c r="BQ50" s="3"/>
-      <c r="BR50" s="3"/>
-      <c r="BS50" s="3"/>
-      <c r="BT50" s="3"/>
-      <c r="BU50" s="3"/>
-      <c r="BV50" s="3"/>
-      <c r="BW50" s="3"/>
-      <c r="BX50" s="3"/>
-      <c r="BY50" s="3"/>
-      <c r="BZ50" s="3"/>
-      <c r="CA50" s="3"/>
-      <c r="CB50" s="3"/>
-      <c r="CC50" s="3"/>
-      <c r="CD50" s="3"/>
-      <c r="CE50" s="3"/>
-      <c r="CF50" s="3"/>
-      <c r="CG50" s="3"/>
-      <c r="CH50" s="3"/>
-      <c r="CI50" s="3"/>
-      <c r="CK50" s="3" t="s">
+      <c r="BD52" s="3"/>
+      <c r="BE52" s="3"/>
+      <c r="BF52" s="3"/>
+      <c r="BG52" s="3"/>
+      <c r="BH52" s="3"/>
+      <c r="BI52" s="3"/>
+      <c r="BJ52" s="3"/>
+      <c r="BK52" s="3"/>
+      <c r="BL52" s="3"/>
+      <c r="BM52" s="3"/>
+      <c r="BN52" s="3"/>
+      <c r="BO52" s="3"/>
+      <c r="BP52" s="3"/>
+      <c r="BQ52" s="3"/>
+      <c r="BR52" s="3"/>
+      <c r="BS52" s="3"/>
+      <c r="BT52" s="3"/>
+      <c r="BU52" s="3"/>
+      <c r="BV52" s="3"/>
+      <c r="BW52" s="3"/>
+      <c r="BX52" s="3"/>
+      <c r="BY52" s="3"/>
+      <c r="BZ52" s="3"/>
+      <c r="CA52" s="3"/>
+      <c r="CB52" s="3"/>
+      <c r="CC52" s="3"/>
+      <c r="CD52" s="3"/>
+      <c r="CE52" s="3"/>
+      <c r="CF52" s="3"/>
+      <c r="CG52" s="3"/>
+      <c r="CH52" s="3"/>
+      <c r="CI52" s="3"/>
+      <c r="CK52" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="CL50" s="3"/>
-      <c r="CM50" s="3"/>
-      <c r="CN50" s="3"/>
-      <c r="CO50" s="3"/>
-      <c r="CP50" s="3"/>
-      <c r="CQ50" s="3"/>
-      <c r="CR50" s="3"/>
-      <c r="CS50" s="3"/>
-      <c r="CT50" s="3"/>
-      <c r="CU50" s="3"/>
-      <c r="CV50" s="3"/>
-      <c r="CW50" s="3"/>
-      <c r="CX50" s="3"/>
-      <c r="CY50" s="3"/>
-      <c r="CZ50" s="3"/>
-      <c r="DA50" s="3"/>
-      <c r="DB50" s="3"/>
-      <c r="DC50" s="3"/>
-      <c r="DD50" s="3"/>
-      <c r="DE50" s="3"/>
-      <c r="DF50" s="3"/>
-      <c r="DG50" s="3"/>
-      <c r="DH50" s="3"/>
-      <c r="DI50" s="3"/>
-      <c r="DJ50" s="3"/>
-      <c r="DK50" s="3"/>
-      <c r="DL50" s="3"/>
-      <c r="DM50" s="3"/>
-      <c r="DN50" s="3"/>
-      <c r="DO50" s="3"/>
-      <c r="DP50" s="3"/>
-      <c r="DQ50" s="3"/>
-      <c r="DR50" s="3"/>
-      <c r="DS50" s="3"/>
-      <c r="DT50" s="3"/>
-      <c r="DU50" s="3"/>
-      <c r="DV50" s="3"/>
-      <c r="DW50" s="3"/>
-      <c r="DX50" s="3"/>
-      <c r="DY50" s="3"/>
-      <c r="DZ50" s="3"/>
-      <c r="EA50" s="3"/>
-      <c r="EB50" s="3"/>
-      <c r="EC50" s="3"/>
-      <c r="ED50" s="3"/>
-      <c r="EE50" s="3"/>
-      <c r="EF50" s="3"/>
-      <c r="EG50" s="3"/>
-      <c r="EH50" s="3"/>
-      <c r="EI50" s="3"/>
-      <c r="EJ50" s="3"/>
-      <c r="EK50" s="3"/>
-      <c r="EL50" s="3"/>
-      <c r="EM50" s="3"/>
-      <c r="EN50" s="3"/>
-      <c r="EO50" s="3"/>
-      <c r="EP50" s="3"/>
-      <c r="EQ50" s="3"/>
-      <c r="ER50" s="3"/>
-      <c r="ES50" s="3"/>
-      <c r="ET50" s="3"/>
-      <c r="EU50" s="3"/>
-      <c r="EV50" s="3"/>
-      <c r="EW50" s="3"/>
-      <c r="EX50" s="3"/>
-      <c r="EY50" s="3"/>
-      <c r="EZ50" s="3"/>
-      <c r="FA50" s="3"/>
-      <c r="FB50" s="3"/>
-      <c r="FC50" s="3"/>
-      <c r="FD50" s="3"/>
-      <c r="FE50" s="3"/>
-      <c r="FF50" s="3"/>
-      <c r="FG50" s="3"/>
-      <c r="FH50" s="3"/>
-      <c r="FI50" s="3"/>
+      <c r="CL52" s="3"/>
+      <c r="CM52" s="3"/>
+      <c r="CN52" s="3"/>
+      <c r="CO52" s="3"/>
+      <c r="CP52" s="3"/>
+      <c r="CQ52" s="3"/>
+      <c r="CR52" s="3"/>
+      <c r="CS52" s="3"/>
+      <c r="CT52" s="3"/>
+      <c r="CU52" s="3"/>
+      <c r="CV52" s="3"/>
+      <c r="CW52" s="3"/>
+      <c r="CX52" s="3"/>
+      <c r="CY52" s="3"/>
+      <c r="CZ52" s="3"/>
+      <c r="DA52" s="3"/>
+      <c r="DB52" s="3"/>
+      <c r="DC52" s="3"/>
+      <c r="DD52" s="3"/>
+      <c r="DE52" s="3"/>
+      <c r="DF52" s="3"/>
+      <c r="DG52" s="3"/>
+      <c r="DH52" s="3"/>
+      <c r="DI52" s="3"/>
+      <c r="DJ52" s="3"/>
+      <c r="DK52" s="3"/>
+      <c r="DL52" s="3"/>
+      <c r="DM52" s="3"/>
+      <c r="DN52" s="3"/>
+      <c r="DO52" s="3"/>
+      <c r="DP52" s="3"/>
+      <c r="DQ52" s="3"/>
+      <c r="DR52" s="3"/>
+      <c r="DS52" s="3"/>
+      <c r="DT52" s="3"/>
+      <c r="DU52" s="3"/>
+      <c r="DV52" s="3"/>
+      <c r="DW52" s="3"/>
+      <c r="DX52" s="3"/>
+      <c r="DY52" s="3"/>
+      <c r="DZ52" s="3"/>
+      <c r="EA52" s="3"/>
+      <c r="EB52" s="3"/>
+      <c r="EC52" s="3"/>
+      <c r="ED52" s="3"/>
+      <c r="EE52" s="3"/>
+      <c r="EF52" s="3"/>
+      <c r="EG52" s="3"/>
+      <c r="EH52" s="3"/>
+      <c r="EI52" s="3"/>
+      <c r="EJ52" s="3"/>
+      <c r="EK52" s="3"/>
+      <c r="EL52" s="3"/>
+      <c r="EM52" s="3"/>
+      <c r="EN52" s="3"/>
+      <c r="EO52" s="3"/>
+      <c r="EP52" s="3"/>
+      <c r="EQ52" s="3"/>
+      <c r="ER52" s="3"/>
+      <c r="ES52" s="3"/>
+      <c r="ET52" s="3"/>
+      <c r="EU52" s="3"/>
+      <c r="EV52" s="3"/>
+      <c r="EW52" s="3"/>
+      <c r="EX52" s="3"/>
+      <c r="EY52" s="3"/>
+      <c r="EZ52" s="3"/>
+      <c r="FA52" s="3"/>
+      <c r="FB52" s="3"/>
+      <c r="FC52" s="3"/>
+      <c r="FD52" s="3"/>
+      <c r="FE52" s="3"/>
+      <c r="FF52" s="3"/>
+      <c r="FG52" s="3"/>
+      <c r="FH52" s="3"/>
+      <c r="FI52" s="3"/>
     </row>
-    <row r="51" spans="21:26" x14ac:dyDescent="0.2">
-      <c r="U51" s="64" t="s">
+    <row r="53" spans="21:26" x14ac:dyDescent="0.2">
+      <c r="U53" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="V51" s="64"/>
-      <c r="W51" s="64"/>
-      <c r="X51" s="64"/>
-      <c r="Y51" s="64"/>
-      <c r="Z51" s="64"/>
+      <c r="V53" s="64"/>
+      <c r="W53" s="64"/>
+      <c r="X53" s="64"/>
+      <c r="Y53" s="64"/>
+      <c r="Z53" s="64"/>
     </row>
   </sheetData>
   <sheetProtection autoFilter="0" deleteColumns="0" deleteRows="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0" insertRows="0" pivotTables="0" sort="0"/>
-  <mergeCells count="1481111111111111111">
+  <mergeCells count="14811111111111111111111111111111111">
     <mergeCell ref="ET31:FI31"/>
     <mergeCell ref="ED31:ES31"/>
     <mergeCell ref="DN31:EC31"/>
@@ -7336,48 +7382,48 @@
     <mergeCell ref="R31:CO31"/>
     <mergeCell ref="I31:Q31"/>
     <mergeCell ref="A31:H31"/>
-    <mergeCell ref="Q50:BA50"/>
-    <mergeCell ref="BC50:CI50"/>
-    <mergeCell ref="CK50:FI50"/>
-    <mergeCell ref="CP42:DM42"/>
-    <mergeCell ref="DN42:EC42"/>
-    <mergeCell ref="ED42:ES42"/>
-    <mergeCell ref="ET42:FI42"/>
-    <mergeCell ref="CP43:DM43"/>
-    <mergeCell ref="DN43:EC43"/>
-    <mergeCell ref="ED43:ES43"/>
-    <mergeCell ref="ET43:FI43"/>
+    <mergeCell ref="Q52:BA52"/>
+    <mergeCell ref="BC52:CI52"/>
+    <mergeCell ref="CK52:FI52"/>
+    <mergeCell ref="CP44:DM44"/>
+    <mergeCell ref="DN44:EC44"/>
+    <mergeCell ref="ED44:ES44"/>
+    <mergeCell ref="ET44:FI44"/>
+    <mergeCell ref="CP45:DM45"/>
+    <mergeCell ref="DN45:EC45"/>
+    <mergeCell ref="ED45:ES45"/>
+    <mergeCell ref="ET45:FI45"/>
     <mergeCell ref="DN35:EC35"/>
     <mergeCell ref="ED35:ES35"/>
     <mergeCell ref="ET35:FI35"/>
-    <mergeCell ref="A41:ES41"/>
-    <mergeCell ref="ET41:FI41"/>
-    <mergeCell ref="U51:Z51"/>
-    <mergeCell ref="U47:Z47"/>
-    <mergeCell ref="I49:P49"/>
-    <mergeCell ref="Q49:BA49"/>
-    <mergeCell ref="BC49:CI49"/>
-    <mergeCell ref="CK49:FI49"/>
-    <mergeCell ref="I45:P45"/>
-    <mergeCell ref="Q45:BA45"/>
-    <mergeCell ref="BC45:CI45"/>
-    <mergeCell ref="CK45:FI45"/>
-    <mergeCell ref="Q46:BA46"/>
-    <mergeCell ref="BC46:CI46"/>
-    <mergeCell ref="CK46:FI46"/>
+    <mergeCell ref="A43:ES43"/>
+    <mergeCell ref="ET43:FI43"/>
+    <mergeCell ref="U53:Z53"/>
+    <mergeCell ref="U49:Z49"/>
+    <mergeCell ref="I51:P51"/>
+    <mergeCell ref="Q51:BA51"/>
+    <mergeCell ref="BC51:CI51"/>
+    <mergeCell ref="CK51:FI51"/>
+    <mergeCell ref="I47:P47"/>
+    <mergeCell ref="Q47:BA47"/>
+    <mergeCell ref="BC47:CI47"/>
+    <mergeCell ref="CK47:FI47"/>
+    <mergeCell ref="Q48:BA48"/>
+    <mergeCell ref="BC48:CI48"/>
+    <mergeCell ref="CK48:FI48"/>
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="I35:Q35"/>
     <mergeCell ref="R35:CO35"/>
     <mergeCell ref="CP35:DA35"/>
     <mergeCell ref="DB35:DM35"/>
-    <mergeCell ref="DN32:EC32"/>
-    <mergeCell ref="ED32:ES32"/>
-    <mergeCell ref="ET32:FI32"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="I32:Q32"/>
-    <mergeCell ref="R32:CO32"/>
-    <mergeCell ref="CP32:DA32"/>
-    <mergeCell ref="DB32:DM32"/>
+    <mergeCell ref="DN33:EC33"/>
+    <mergeCell ref="ED33:ES33"/>
+    <mergeCell ref="ET33:FI33"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:Q33"/>
+    <mergeCell ref="R33:CO33"/>
+    <mergeCell ref="CP33:DA33"/>
+    <mergeCell ref="DB33:DM33"/>
     <mergeCell ref="A30:FI30"/>
     <mergeCell ref="DN27:EC28"/>
     <mergeCell ref="ED27:ES28"/>
@@ -7460,6 +7506,14 @@
     <mergeCell ref="DN38:EC38"/>
     <mergeCell ref="ED38:ES38"/>
     <mergeCell ref="ET38:FI38"/>
+    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="I42:Q42"/>
+    <mergeCell ref="R42:CO42"/>
+    <mergeCell ref="CP42:DA42"/>
+    <mergeCell ref="DB42:DM42"/>
+    <mergeCell ref="DN42:EC42"/>
+    <mergeCell ref="ED42:ES42"/>
+    <mergeCell ref="ET42:FI42"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="I40:Q40"/>
     <mergeCell ref="R40:CO40"/>
@@ -7468,6 +7522,22 @@
     <mergeCell ref="DN40:EC40"/>
     <mergeCell ref="ED40:ES40"/>
     <mergeCell ref="ET40:FI40"/>
+    <mergeCell ref="ET32:FI32"/>
+    <mergeCell ref="ED32:ES32"/>
+    <mergeCell ref="DN32:EC32"/>
+    <mergeCell ref="DB32:DM32"/>
+    <mergeCell ref="CP32:DA32"/>
+    <mergeCell ref="R32:CO32"/>
+    <mergeCell ref="I32:Q32"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="DN34:EC34"/>
+    <mergeCell ref="ED34:ES34"/>
+    <mergeCell ref="ET34:FI34"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="I34:Q34"/>
+    <mergeCell ref="R34:CO34"/>
+    <mergeCell ref="CP34:DA34"/>
+    <mergeCell ref="DB34:DM34"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="I39:Q39"/>
     <mergeCell ref="R39:CO39"/>
@@ -7476,22 +7546,14 @@
     <mergeCell ref="DN39:EC39"/>
     <mergeCell ref="ED39:ES39"/>
     <mergeCell ref="ET39:FI39"/>
-    <mergeCell ref="DN33:EC33"/>
-    <mergeCell ref="DN34:EC34"/>
-    <mergeCell ref="ED33:ES33"/>
-    <mergeCell ref="ED34:ES34"/>
-    <mergeCell ref="ET33:FI33"/>
-    <mergeCell ref="ET34:FI34"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="I33:Q33"/>
-    <mergeCell ref="I34:Q34"/>
-    <mergeCell ref="R33:CO33"/>
-    <mergeCell ref="R34:CO34"/>
-    <mergeCell ref="CP33:DA33"/>
-    <mergeCell ref="CP34:DA34"/>
-    <mergeCell ref="DB33:DM33"/>
-    <mergeCell ref="DB34:DM34"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="I41:Q41"/>
+    <mergeCell ref="R41:CO41"/>
+    <mergeCell ref="CP41:DA41"/>
+    <mergeCell ref="DB41:DM41"/>
+    <mergeCell ref="DN41:EC41"/>
+    <mergeCell ref="ED41:ES41"/>
+    <mergeCell ref="ET41:FI41"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.5" footer="0.3" header="0.3" left="0.75" right="0.75" top="0.5"/>

</xml_diff>